<commit_message>
error handling and previous commit changes added to lambda handlers
</commit_message>
<xml_diff>
--- a/database/Sparrows.xlsx
+++ b/database/Sparrows.xlsx
@@ -1033,7 +1033,7 @@
       </c>
       <c r="R11" t="inlineStr">
         <is>
-          <t>['Manufacturer not found']</t>
+          <t>['Manufacturer not found', 'page no: 8']</t>
         </is>
       </c>
     </row>
@@ -1081,7 +1081,7 @@
       </c>
       <c r="R12" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'Model not found']</t>
+          <t>['Manufacturer not found', 'Model not found', 'page no: 9']</t>
         </is>
       </c>
     </row>
@@ -1129,7 +1129,7 @@
       </c>
       <c r="R13" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'Model not found']</t>
+          <t>['Manufacturer not found', 'Model not found', 'page no: 10']</t>
         </is>
       </c>
     </row>
@@ -1879,7 +1879,7 @@
       </c>
       <c r="R27" t="inlineStr">
         <is>
-          <t>['Model not found']</t>
+          <t>['Model not found', 'page no: 24']</t>
         </is>
       </c>
     </row>
@@ -1936,7 +1936,7 @@
       </c>
       <c r="R28" t="inlineStr">
         <is>
-          <t>['Manufacturer not found']</t>
+          <t>['Manufacturer not found', 'page no: 25']</t>
         </is>
       </c>
     </row>
@@ -2094,7 +2094,7 @@
       </c>
       <c r="R31" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'Model not found']</t>
+          <t>['Manufacturer not found', 'Model not found', 'page no: 28']</t>
         </is>
       </c>
     </row>
@@ -2147,7 +2147,7 @@
       </c>
       <c r="R32" t="inlineStr">
         <is>
-          <t>['Manufacturer not found']</t>
+          <t>['Manufacturer not found', 'page no: 29']</t>
         </is>
       </c>
     </row>
@@ -2200,7 +2200,7 @@
       </c>
       <c r="R33" t="inlineStr">
         <is>
-          <t>['Manufacturer not found']</t>
+          <t>['Manufacturer not found', 'page no: 29']</t>
         </is>
       </c>
     </row>
@@ -2253,7 +2253,7 @@
       </c>
       <c r="R34" t="inlineStr">
         <is>
-          <t>['Manufacturer not found']</t>
+          <t>['Manufacturer not found', 'page no: 29']</t>
         </is>
       </c>
     </row>
@@ -2306,7 +2306,7 @@
       </c>
       <c r="R35" t="inlineStr">
         <is>
-          <t>['Manufacturer not found']</t>
+          <t>['Manufacturer not found', 'page no: 29']</t>
         </is>
       </c>
     </row>
@@ -2359,7 +2359,7 @@
       </c>
       <c r="R36" t="inlineStr">
         <is>
-          <t>['Manufacturer not found']</t>
+          <t>['Manufacturer not found', 'page no: 29']</t>
         </is>
       </c>
     </row>
@@ -2412,7 +2412,7 @@
       </c>
       <c r="R37" t="inlineStr">
         <is>
-          <t>['Manufacturer not found']</t>
+          <t>['Manufacturer not found', 'page no: 29']</t>
         </is>
       </c>
     </row>
@@ -2465,7 +2465,7 @@
       </c>
       <c r="R38" t="inlineStr">
         <is>
-          <t>['Manufacturer not found']</t>
+          <t>['Manufacturer not found', 'page no: 30']</t>
         </is>
       </c>
     </row>
@@ -2518,7 +2518,7 @@
       </c>
       <c r="R39" t="inlineStr">
         <is>
-          <t>['Manufacturer not found']</t>
+          <t>['Manufacturer not found', 'page no: 30']</t>
         </is>
       </c>
     </row>
@@ -2572,7 +2572,7 @@
       </c>
       <c r="R40" t="inlineStr">
         <is>
-          <t>['Manufacturer not found']</t>
+          <t>['Manufacturer not found', 'page no: 30']</t>
         </is>
       </c>
     </row>
@@ -2625,7 +2625,7 @@
       </c>
       <c r="R41" t="inlineStr">
         <is>
-          <t>['Manufacturer not found']</t>
+          <t>['Manufacturer not found', 'page no: 30']</t>
         </is>
       </c>
     </row>
@@ -2678,7 +2678,7 @@
       </c>
       <c r="R42" t="inlineStr">
         <is>
-          <t>['Manufacturer not found']</t>
+          <t>['Manufacturer not found', 'page no: 30']</t>
         </is>
       </c>
     </row>
@@ -2731,7 +2731,7 @@
       </c>
       <c r="R43" t="inlineStr">
         <is>
-          <t>['Manufacturer not found']</t>
+          <t>['Manufacturer not found', 'page no: 30']</t>
         </is>
       </c>
     </row>
@@ -2784,7 +2784,7 @@
       </c>
       <c r="R44" t="inlineStr">
         <is>
-          <t>['Model not found']</t>
+          <t>['Model not found', 'page no: 31']</t>
         </is>
       </c>
     </row>
@@ -2837,7 +2837,7 @@
       </c>
       <c r="R45" t="inlineStr">
         <is>
-          <t>['Model not found']</t>
+          <t>['Model not found', 'page no: 31']</t>
         </is>
       </c>
     </row>
@@ -2890,7 +2890,7 @@
       </c>
       <c r="R46" t="inlineStr">
         <is>
-          <t>['Model not found']</t>
+          <t>['Model not found', 'page no: 32']</t>
         </is>
       </c>
     </row>
@@ -2943,7 +2943,7 @@
       </c>
       <c r="R47" t="inlineStr">
         <is>
-          <t>['Model not found']</t>
+          <t>['Model not found', 'page no: 32']</t>
         </is>
       </c>
     </row>
@@ -2996,7 +2996,7 @@
       </c>
       <c r="R48" t="inlineStr">
         <is>
-          <t>['Model not found']</t>
+          <t>['Model not found', 'page no: 32']</t>
         </is>
       </c>
     </row>
@@ -3049,7 +3049,7 @@
       </c>
       <c r="R49" t="inlineStr">
         <is>
-          <t>['Model not found']</t>
+          <t>['Model not found', 'page no: 32']</t>
         </is>
       </c>
     </row>
@@ -3102,7 +3102,7 @@
       </c>
       <c r="R50" t="inlineStr">
         <is>
-          <t>['Model not found']</t>
+          <t>['Model not found', 'page no: 32']</t>
         </is>
       </c>
     </row>
@@ -3155,7 +3155,7 @@
       </c>
       <c r="R51" t="inlineStr">
         <is>
-          <t>['Model not found']</t>
+          <t>['Model not found', 'page no: 32']</t>
         </is>
       </c>
     </row>
@@ -3208,7 +3208,7 @@
       </c>
       <c r="R52" t="inlineStr">
         <is>
-          <t>['Model not found']</t>
+          <t>['Model not found', 'page no: 32']</t>
         </is>
       </c>
     </row>
@@ -3261,7 +3261,7 @@
       </c>
       <c r="R53" t="inlineStr">
         <is>
-          <t>['Model not found']</t>
+          <t>['Model not found', 'page no: 32']</t>
         </is>
       </c>
     </row>
@@ -3314,7 +3314,7 @@
       </c>
       <c r="R54" t="inlineStr">
         <is>
-          <t>['Model not found']</t>
+          <t>['Model not found', 'page no: 32']</t>
         </is>
       </c>
     </row>
@@ -3367,7 +3367,7 @@
       </c>
       <c r="R55" t="inlineStr">
         <is>
-          <t>['Model not found']</t>
+          <t>['Model not found', 'page no: 32']</t>
         </is>
       </c>
     </row>
@@ -3420,7 +3420,7 @@
       </c>
       <c r="R56" t="inlineStr">
         <is>
-          <t>['Model not found']</t>
+          <t>['Model not found', 'page no: 32']</t>
         </is>
       </c>
     </row>
@@ -3473,7 +3473,7 @@
       </c>
       <c r="R57" t="inlineStr">
         <is>
-          <t>['Model not found']</t>
+          <t>['Model not found', 'page no: 32']</t>
         </is>
       </c>
     </row>
@@ -3526,7 +3526,7 @@
       </c>
       <c r="R58" t="inlineStr">
         <is>
-          <t>['Model not found']</t>
+          <t>['Model not found', 'page no: 33']</t>
         </is>
       </c>
     </row>
@@ -3579,7 +3579,7 @@
       </c>
       <c r="R59" t="inlineStr">
         <is>
-          <t>['Model not found']</t>
+          <t>['Model not found', 'page no: 33']</t>
         </is>
       </c>
     </row>
@@ -3632,7 +3632,7 @@
       </c>
       <c r="R60" t="inlineStr">
         <is>
-          <t>['Model not found']</t>
+          <t>['Model not found', 'page no: 33']</t>
         </is>
       </c>
     </row>
@@ -3685,7 +3685,7 @@
       </c>
       <c r="R61" t="inlineStr">
         <is>
-          <t>['Model not found']</t>
+          <t>['Model not found', 'page no: 33']</t>
         </is>
       </c>
     </row>
@@ -3738,7 +3738,7 @@
       </c>
       <c r="R62" t="inlineStr">
         <is>
-          <t>['Model not found']</t>
+          <t>['Model not found', 'page no: 33']</t>
         </is>
       </c>
     </row>
@@ -3791,7 +3791,7 @@
       </c>
       <c r="R63" t="inlineStr">
         <is>
-          <t>['Model not found']</t>
+          <t>['Model not found', 'page no: 33']</t>
         </is>
       </c>
     </row>
@@ -3844,7 +3844,7 @@
       </c>
       <c r="R64" t="inlineStr">
         <is>
-          <t>['Model not found']</t>
+          <t>['Model not found', 'page no: 33']</t>
         </is>
       </c>
     </row>
@@ -3897,7 +3897,7 @@
       </c>
       <c r="R65" t="inlineStr">
         <is>
-          <t>['Model not found']</t>
+          <t>['Model not found', 'page no: 33']</t>
         </is>
       </c>
     </row>
@@ -3950,7 +3950,7 @@
       </c>
       <c r="R66" t="inlineStr">
         <is>
-          <t>['Model not found']</t>
+          <t>['Model not found', 'page no: 34']</t>
         </is>
       </c>
     </row>
@@ -4003,7 +4003,7 @@
       </c>
       <c r="R67" t="inlineStr">
         <is>
-          <t>['Model not found']</t>
+          <t>['Model not found', 'page no: 34']</t>
         </is>
       </c>
     </row>
@@ -4056,7 +4056,7 @@
       </c>
       <c r="R68" t="inlineStr">
         <is>
-          <t>['Model not found']</t>
+          <t>['Model not found', 'page no: 34']</t>
         </is>
       </c>
     </row>
@@ -4109,7 +4109,7 @@
       </c>
       <c r="R69" t="inlineStr">
         <is>
-          <t>['Model not found']</t>
+          <t>['Model not found', 'page no: 34']</t>
         </is>
       </c>
     </row>
@@ -4162,7 +4162,7 @@
       </c>
       <c r="R70" t="inlineStr">
         <is>
-          <t>['Manufacturer not found']</t>
+          <t>['Manufacturer not found', 'page no: 35']</t>
         </is>
       </c>
     </row>
@@ -4215,7 +4215,7 @@
       </c>
       <c r="R71" t="inlineStr">
         <is>
-          <t>['Manufacturer not found']</t>
+          <t>['Manufacturer not found', 'page no: 35']</t>
         </is>
       </c>
     </row>
@@ -4268,7 +4268,7 @@
       </c>
       <c r="R72" t="inlineStr">
         <is>
-          <t>['Manufacturer not found']</t>
+          <t>['Manufacturer not found', 'page no: 35']</t>
         </is>
       </c>
     </row>
@@ -4321,7 +4321,7 @@
       </c>
       <c r="R73" t="inlineStr">
         <is>
-          <t>['Manufacturer not found']</t>
+          <t>['Manufacturer not found', 'page no: 35']</t>
         </is>
       </c>
     </row>
@@ -4374,7 +4374,7 @@
       </c>
       <c r="R74" t="inlineStr">
         <is>
-          <t>['Manufacturer not found']</t>
+          <t>['Manufacturer not found', 'page no: 35']</t>
         </is>
       </c>
     </row>
@@ -4427,7 +4427,7 @@
       </c>
       <c r="R75" t="inlineStr">
         <is>
-          <t>['Manufacturer not found']</t>
+          <t>['Manufacturer not found', 'page no: 35']</t>
         </is>
       </c>
     </row>
@@ -4480,7 +4480,7 @@
       </c>
       <c r="R76" t="inlineStr">
         <is>
-          <t>['Manufacturer not found']</t>
+          <t>['Manufacturer not found', 'page no: 35']</t>
         </is>
       </c>
     </row>
@@ -4533,7 +4533,7 @@
       </c>
       <c r="R77" t="inlineStr">
         <is>
-          <t>['Manufacturer not found']</t>
+          <t>['Manufacturer not found', 'page no: 35']</t>
         </is>
       </c>
     </row>
@@ -4586,7 +4586,7 @@
       </c>
       <c r="R78" t="inlineStr">
         <is>
-          <t>['Manufacturer not found']</t>
+          <t>['Manufacturer not found', 'page no: 35']</t>
         </is>
       </c>
     </row>
@@ -4639,7 +4639,7 @@
       </c>
       <c r="R79" t="inlineStr">
         <is>
-          <t>['Manufacturer not found']</t>
+          <t>['Manufacturer not found', 'page no: 35']</t>
         </is>
       </c>
     </row>
@@ -4692,7 +4692,7 @@
       </c>
       <c r="R80" t="inlineStr">
         <is>
-          <t>['Manufacturer not found']</t>
+          <t>['Manufacturer not found', 'page no: 35']</t>
         </is>
       </c>
     </row>
@@ -4745,7 +4745,7 @@
       </c>
       <c r="R81" t="inlineStr">
         <is>
-          <t>['Manufacturer not found']</t>
+          <t>['Manufacturer not found', 'page no: 35']</t>
         </is>
       </c>
     </row>
@@ -4798,7 +4798,7 @@
       </c>
       <c r="R82" t="inlineStr">
         <is>
-          <t>['Manufacturer not found']</t>
+          <t>['Manufacturer not found', 'page no: 35']</t>
         </is>
       </c>
     </row>
@@ -4851,7 +4851,7 @@
       </c>
       <c r="R83" t="inlineStr">
         <is>
-          <t>['Manufacturer not found']</t>
+          <t>['Manufacturer not found', 'page no: 35']</t>
         </is>
       </c>
     </row>
@@ -4904,7 +4904,7 @@
       </c>
       <c r="R84" t="inlineStr">
         <is>
-          <t>['Manufacturer not found']</t>
+          <t>['Manufacturer not found', 'page no: 35']</t>
         </is>
       </c>
     </row>
@@ -4957,7 +4957,7 @@
       </c>
       <c r="R85" t="inlineStr">
         <is>
-          <t>['Manufacturer not found']</t>
+          <t>['Manufacturer not found', 'page no: 35']</t>
         </is>
       </c>
     </row>
@@ -5010,7 +5010,7 @@
       </c>
       <c r="R86" t="inlineStr">
         <is>
-          <t>['Manufacturer not found']</t>
+          <t>['Manufacturer not found', 'page no: 35']</t>
         </is>
       </c>
     </row>
@@ -5063,7 +5063,7 @@
       </c>
       <c r="R87" t="inlineStr">
         <is>
-          <t>['Manufacturer not found']</t>
+          <t>['Manufacturer not found', 'page no: 35']</t>
         </is>
       </c>
     </row>
@@ -5116,7 +5116,7 @@
       </c>
       <c r="R88" t="inlineStr">
         <is>
-          <t>['Manufacturer not found']</t>
+          <t>['Manufacturer not found', 'page no: 35']</t>
         </is>
       </c>
     </row>
@@ -5169,7 +5169,7 @@
       </c>
       <c r="R89" t="inlineStr">
         <is>
-          <t>['Manufacturer not found']</t>
+          <t>['Manufacturer not found', 'page no: 35']</t>
         </is>
       </c>
     </row>
@@ -5222,7 +5222,7 @@
       </c>
       <c r="R90" t="inlineStr">
         <is>
-          <t>['Manufacturer not found']</t>
+          <t>['Manufacturer not found', 'page no: 35']</t>
         </is>
       </c>
     </row>
@@ -5275,7 +5275,7 @@
       </c>
       <c r="R91" t="inlineStr">
         <is>
-          <t>['Manufacturer not found']</t>
+          <t>['Manufacturer not found', 'page no: 35']</t>
         </is>
       </c>
     </row>
@@ -5328,7 +5328,7 @@
       </c>
       <c r="R92" t="inlineStr">
         <is>
-          <t>['Manufacturer not found']</t>
+          <t>['Manufacturer not found', 'page no: 35']</t>
         </is>
       </c>
     </row>
@@ -5381,7 +5381,7 @@
       </c>
       <c r="R93" t="inlineStr">
         <is>
-          <t>['Manufacturer not found']</t>
+          <t>['Manufacturer not found', 'page no: 35']</t>
         </is>
       </c>
     </row>
@@ -5434,7 +5434,7 @@
       </c>
       <c r="R94" t="inlineStr">
         <is>
-          <t>['Manufacturer not found']</t>
+          <t>['Manufacturer not found', 'page no: 35']</t>
         </is>
       </c>
     </row>
@@ -5487,7 +5487,7 @@
       </c>
       <c r="R95" t="inlineStr">
         <is>
-          <t>['Manufacturer not found']</t>
+          <t>['Manufacturer not found', 'page no: 35']</t>
         </is>
       </c>
     </row>
@@ -5540,7 +5540,7 @@
       </c>
       <c r="R96" t="inlineStr">
         <is>
-          <t>['Manufacturer not found']</t>
+          <t>['Manufacturer not found', 'page no: 35']</t>
         </is>
       </c>
     </row>
@@ -5593,7 +5593,7 @@
       </c>
       <c r="R97" t="inlineStr">
         <is>
-          <t>['Manufacturer not found']</t>
+          <t>['Manufacturer not found', 'page no: 35']</t>
         </is>
       </c>
     </row>
@@ -5646,7 +5646,7 @@
       </c>
       <c r="R98" t="inlineStr">
         <is>
-          <t>['Manufacturer not found']</t>
+          <t>['Manufacturer not found', 'page no: 35']</t>
         </is>
       </c>
     </row>
@@ -5699,7 +5699,7 @@
       </c>
       <c r="R99" t="inlineStr">
         <is>
-          <t>['Manufacturer not found']</t>
+          <t>['Manufacturer not found', 'page no: 35']</t>
         </is>
       </c>
     </row>
@@ -5752,7 +5752,7 @@
       </c>
       <c r="R100" t="inlineStr">
         <is>
-          <t>['Manufacturer not found']</t>
+          <t>['Manufacturer not found', 'page no: 35']</t>
         </is>
       </c>
     </row>
@@ -5805,7 +5805,7 @@
       </c>
       <c r="R101" t="inlineStr">
         <is>
-          <t>['Manufacturer not found']</t>
+          <t>['Manufacturer not found', 'page no: 35']</t>
         </is>
       </c>
     </row>
@@ -5858,7 +5858,7 @@
       </c>
       <c r="R102" t="inlineStr">
         <is>
-          <t>['Manufacturer not found']</t>
+          <t>['Manufacturer not found', 'page no: 35']</t>
         </is>
       </c>
     </row>
@@ -5911,7 +5911,7 @@
       </c>
       <c r="R103" t="inlineStr">
         <is>
-          <t>['Manufacturer not found']</t>
+          <t>['Manufacturer not found', 'page no: 35']</t>
         </is>
       </c>
     </row>
@@ -5964,7 +5964,7 @@
       </c>
       <c r="R104" t="inlineStr">
         <is>
-          <t>['Manufacturer not found']</t>
+          <t>['Manufacturer not found', 'page no: 35']</t>
         </is>
       </c>
     </row>
@@ -6017,7 +6017,7 @@
       </c>
       <c r="R105" t="inlineStr">
         <is>
-          <t>['Manufacturer not found']</t>
+          <t>['Manufacturer not found', 'page no: 35']</t>
         </is>
       </c>
     </row>
@@ -6065,7 +6065,7 @@
       </c>
       <c r="R106" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'Model not found']</t>
+          <t>['Manufacturer not found', 'Model not found', 'page no: 36']</t>
         </is>
       </c>
     </row>
@@ -6113,7 +6113,7 @@
       </c>
       <c r="R107" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'Model not found']</t>
+          <t>['Manufacturer not found', 'Model not found', 'page no: 36']</t>
         </is>
       </c>
     </row>
@@ -6161,7 +6161,7 @@
       </c>
       <c r="R108" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'Model not found']</t>
+          <t>['Manufacturer not found', 'Model not found', 'page no: 36']</t>
         </is>
       </c>
     </row>
@@ -6209,7 +6209,7 @@
       </c>
       <c r="R109" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'Model not found']</t>
+          <t>['Manufacturer not found', 'Model not found', 'page no: 36']</t>
         </is>
       </c>
     </row>
@@ -6257,7 +6257,7 @@
       </c>
       <c r="R110" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'Model not found']</t>
+          <t>['Manufacturer not found', 'Model not found', 'page no: 36']</t>
         </is>
       </c>
     </row>
@@ -6305,7 +6305,7 @@
       </c>
       <c r="R111" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'Model not found']</t>
+          <t>['Manufacturer not found', 'Model not found', 'page no: 36']</t>
         </is>
       </c>
     </row>
@@ -6358,7 +6358,7 @@
       </c>
       <c r="R112" t="inlineStr">
         <is>
-          <t>['Manufacturer not found']</t>
+          <t>['Manufacturer not found', 'page no: 37']</t>
         </is>
       </c>
     </row>
@@ -6411,7 +6411,7 @@
       </c>
       <c r="R113" t="inlineStr">
         <is>
-          <t>['Manufacturer not found']</t>
+          <t>['Manufacturer not found', 'page no: 37']</t>
         </is>
       </c>
     </row>
@@ -6464,7 +6464,7 @@
       </c>
       <c r="R114" t="inlineStr">
         <is>
-          <t>['Manufacturer not found']</t>
+          <t>['Manufacturer not found', 'page no: 37']</t>
         </is>
       </c>
     </row>
@@ -6517,7 +6517,7 @@
       </c>
       <c r="R115" t="inlineStr">
         <is>
-          <t>['Manufacturer not found']</t>
+          <t>['Manufacturer not found', 'page no: 37']</t>
         </is>
       </c>
     </row>
@@ -6570,7 +6570,7 @@
       </c>
       <c r="R116" t="inlineStr">
         <is>
-          <t>['Manufacturer not found']</t>
+          <t>['Manufacturer not found', 'page no: 37']</t>
         </is>
       </c>
     </row>
@@ -6623,7 +6623,7 @@
       </c>
       <c r="R117" t="inlineStr">
         <is>
-          <t>['Manufacturer not found']</t>
+          <t>['Manufacturer not found', 'page no: 37']</t>
         </is>
       </c>
     </row>
@@ -6676,7 +6676,7 @@
       </c>
       <c r="R118" t="inlineStr">
         <is>
-          <t>['Manufacturer not found']</t>
+          <t>['Manufacturer not found', 'page no: 37']</t>
         </is>
       </c>
     </row>
@@ -6729,7 +6729,7 @@
       </c>
       <c r="R119" t="inlineStr">
         <is>
-          <t>['Manufacturer not found']</t>
+          <t>['Manufacturer not found', 'page no: 37']</t>
         </is>
       </c>
     </row>
@@ -6782,7 +6782,7 @@
       </c>
       <c r="R120" t="inlineStr">
         <is>
-          <t>['Manufacturer not found']</t>
+          <t>['Manufacturer not found', 'page no: 37']</t>
         </is>
       </c>
     </row>
@@ -6835,7 +6835,7 @@
       </c>
       <c r="R121" t="inlineStr">
         <is>
-          <t>['Manufacturer not found']</t>
+          <t>['Manufacturer not found', 'page no: 37']</t>
         </is>
       </c>
     </row>
@@ -6883,7 +6883,7 @@
       </c>
       <c r="R122" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'Model not found']</t>
+          <t>['Manufacturer not found', 'Model not found', 'page no: 38']</t>
         </is>
       </c>
     </row>
@@ -6931,7 +6931,7 @@
       </c>
       <c r="R123" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'Model not found']</t>
+          <t>['Manufacturer not found', 'Model not found', 'page no: 38']</t>
         </is>
       </c>
     </row>
@@ -6979,7 +6979,7 @@
       </c>
       <c r="R124" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'Model not found']</t>
+          <t>['Manufacturer not found', 'Model not found', 'page no: 38']</t>
         </is>
       </c>
     </row>
@@ -7027,7 +7027,7 @@
       </c>
       <c r="R125" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'Model not found']</t>
+          <t>['Manufacturer not found', 'Model not found', 'page no: 38']</t>
         </is>
       </c>
     </row>
@@ -7075,7 +7075,7 @@
       </c>
       <c r="R126" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'Model not found']</t>
+          <t>['Manufacturer not found', 'Model not found', 'page no: 38']</t>
         </is>
       </c>
     </row>
@@ -7123,7 +7123,7 @@
       </c>
       <c r="R127" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'Model not found']</t>
+          <t>['Manufacturer not found', 'Model not found', 'page no: 38']</t>
         </is>
       </c>
     </row>
@@ -7171,7 +7171,7 @@
       </c>
       <c r="R128" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'Model not found']</t>
+          <t>['Manufacturer not found', 'Model not found', 'page no: 39']</t>
         </is>
       </c>
     </row>
@@ -7219,7 +7219,7 @@
       </c>
       <c r="R129" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'Model not found']</t>
+          <t>['Manufacturer not found', 'Model not found', 'page no: 39']</t>
         </is>
       </c>
     </row>
@@ -7267,7 +7267,7 @@
       </c>
       <c r="R130" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'Model not found']</t>
+          <t>['Manufacturer not found', 'Model not found', 'page no: 39']</t>
         </is>
       </c>
     </row>
@@ -7315,7 +7315,7 @@
       </c>
       <c r="R131" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'Model not found']</t>
+          <t>['Manufacturer not found', 'Model not found', 'page no: 39']</t>
         </is>
       </c>
     </row>
@@ -7474,7 +7474,7 @@
       </c>
       <c r="R134" t="inlineStr">
         <is>
-          <t>['Model not found']</t>
+          <t>['Model not found', 'page no: 41']</t>
         </is>
       </c>
     </row>
@@ -7516,7 +7516,7 @@
       </c>
       <c r="R135" t="inlineStr">
         <is>
-          <t>['Model not found', 'SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty']</t>
+          <t>['Model not found', 'SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 42']</t>
         </is>
       </c>
     </row>
@@ -7559,7 +7559,7 @@
       </c>
       <c r="R136" t="inlineStr">
         <is>
-          <t>['Model not found', 'SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty']</t>
+          <t>['Model not found', 'SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 42']</t>
         </is>
       </c>
     </row>
@@ -7601,7 +7601,7 @@
       </c>
       <c r="R137" t="inlineStr">
         <is>
-          <t>['Model not found', 'SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty']</t>
+          <t>['Model not found', 'SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 42']</t>
         </is>
       </c>
     </row>
@@ -7644,7 +7644,7 @@
       </c>
       <c r="R138" t="inlineStr">
         <is>
-          <t>['Model not found', 'SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty']</t>
+          <t>['Model not found', 'SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 42']</t>
         </is>
       </c>
     </row>
@@ -7691,7 +7691,7 @@
       </c>
       <c r="R139" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty']</t>
+          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 43']</t>
         </is>
       </c>
     </row>
@@ -7738,7 +7738,7 @@
       </c>
       <c r="R140" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty']</t>
+          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 43']</t>
         </is>
       </c>
     </row>
@@ -7785,7 +7785,7 @@
       </c>
       <c r="R141" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty']</t>
+          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 43']</t>
         </is>
       </c>
     </row>
@@ -7832,7 +7832,7 @@
       </c>
       <c r="R142" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty']</t>
+          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 43']</t>
         </is>
       </c>
     </row>
@@ -7879,7 +7879,7 @@
       </c>
       <c r="R143" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty']</t>
+          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 43']</t>
         </is>
       </c>
     </row>
@@ -7926,7 +7926,7 @@
       </c>
       <c r="R144" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty']</t>
+          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 43']</t>
         </is>
       </c>
     </row>
@@ -7973,7 +7973,7 @@
       </c>
       <c r="R145" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty']</t>
+          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 43']</t>
         </is>
       </c>
     </row>
@@ -8020,7 +8020,7 @@
       </c>
       <c r="R146" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty']</t>
+          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 43']</t>
         </is>
       </c>
     </row>
@@ -8067,7 +8067,7 @@
       </c>
       <c r="R147" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty']</t>
+          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 43']</t>
         </is>
       </c>
     </row>
@@ -8114,7 +8114,7 @@
       </c>
       <c r="R148" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty']</t>
+          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 43']</t>
         </is>
       </c>
     </row>
@@ -8161,7 +8161,7 @@
       </c>
       <c r="R149" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty']</t>
+          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 43']</t>
         </is>
       </c>
     </row>
@@ -8208,7 +8208,7 @@
       </c>
       <c r="R150" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty']</t>
+          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 43']</t>
         </is>
       </c>
     </row>
@@ -8255,7 +8255,7 @@
       </c>
       <c r="R151" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty']</t>
+          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 43']</t>
         </is>
       </c>
     </row>
@@ -8302,7 +8302,7 @@
       </c>
       <c r="R152" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty']</t>
+          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 43']</t>
         </is>
       </c>
     </row>
@@ -8349,7 +8349,7 @@
       </c>
       <c r="R153" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty']</t>
+          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 43']</t>
         </is>
       </c>
     </row>
@@ -8396,7 +8396,7 @@
       </c>
       <c r="R154" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty']</t>
+          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 43']</t>
         </is>
       </c>
     </row>
@@ -8443,7 +8443,7 @@
       </c>
       <c r="R155" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty']</t>
+          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 43']</t>
         </is>
       </c>
     </row>
@@ -8490,7 +8490,7 @@
       </c>
       <c r="R156" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty']</t>
+          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 43']</t>
         </is>
       </c>
     </row>
@@ -8537,7 +8537,7 @@
       </c>
       <c r="R157" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty']</t>
+          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 43']</t>
         </is>
       </c>
     </row>
@@ -8584,7 +8584,7 @@
       </c>
       <c r="R158" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty']</t>
+          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 43']</t>
         </is>
       </c>
     </row>
@@ -8631,7 +8631,7 @@
       </c>
       <c r="R159" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty']</t>
+          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 43']</t>
         </is>
       </c>
     </row>
@@ -8678,7 +8678,7 @@
       </c>
       <c r="R160" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty']</t>
+          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 43']</t>
         </is>
       </c>
     </row>
@@ -8725,7 +8725,7 @@
       </c>
       <c r="R161" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty']</t>
+          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 43']</t>
         </is>
       </c>
     </row>
@@ -8772,7 +8772,7 @@
       </c>
       <c r="R162" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty']</t>
+          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 43']</t>
         </is>
       </c>
     </row>
@@ -8822,7 +8822,7 @@
       </c>
       <c r="R163" t="inlineStr">
         <is>
-          <t>['SWL Value not found', 'SWL Unit not found']</t>
+          <t>['SWL Value not found', 'SWL Unit not found', 'page no: 44']</t>
         </is>
       </c>
     </row>
@@ -8873,7 +8873,7 @@
       </c>
       <c r="R164" t="inlineStr">
         <is>
-          <t>['SWL Value not found', 'SWL Unit not found']</t>
+          <t>['SWL Value not found', 'SWL Unit not found', 'page no: 44']</t>
         </is>
       </c>
     </row>
@@ -8924,7 +8924,7 @@
       </c>
       <c r="R165" t="inlineStr">
         <is>
-          <t>['SWL Value not found', 'SWL Unit not found']</t>
+          <t>['SWL Value not found', 'SWL Unit not found', 'page no: 44']</t>
         </is>
       </c>
     </row>
@@ -8975,7 +8975,7 @@
       </c>
       <c r="R166" t="inlineStr">
         <is>
-          <t>['SWL Value not found', 'SWL Unit not found']</t>
+          <t>['SWL Value not found', 'SWL Unit not found', 'page no: 44']</t>
         </is>
       </c>
     </row>
@@ -9022,7 +9022,7 @@
       </c>
       <c r="R167" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty']</t>
+          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 45']</t>
         </is>
       </c>
     </row>
@@ -9069,7 +9069,7 @@
       </c>
       <c r="R168" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty']</t>
+          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 45']</t>
         </is>
       </c>
     </row>
@@ -9116,7 +9116,7 @@
       </c>
       <c r="R169" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty']</t>
+          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 45']</t>
         </is>
       </c>
     </row>
@@ -9163,7 +9163,7 @@
       </c>
       <c r="R170" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty']</t>
+          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 45']</t>
         </is>
       </c>
     </row>
@@ -9210,7 +9210,7 @@
       </c>
       <c r="R171" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty']</t>
+          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 45']</t>
         </is>
       </c>
     </row>
@@ -9257,7 +9257,7 @@
       </c>
       <c r="R172" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty']</t>
+          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 45']</t>
         </is>
       </c>
     </row>
@@ -9304,7 +9304,7 @@
       </c>
       <c r="R173" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty']</t>
+          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 45']</t>
         </is>
       </c>
     </row>
@@ -9351,7 +9351,7 @@
       </c>
       <c r="R174" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty']</t>
+          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 45']</t>
         </is>
       </c>
     </row>
@@ -9398,7 +9398,7 @@
       </c>
       <c r="R175" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty']</t>
+          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 45']</t>
         </is>
       </c>
     </row>
@@ -9445,7 +9445,7 @@
       </c>
       <c r="R176" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty']</t>
+          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 45']</t>
         </is>
       </c>
     </row>
@@ -9492,7 +9492,7 @@
       </c>
       <c r="R177" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty']</t>
+          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 45']</t>
         </is>
       </c>
     </row>
@@ -9539,7 +9539,7 @@
       </c>
       <c r="R178" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty']</t>
+          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 45']</t>
         </is>
       </c>
     </row>
@@ -9586,7 +9586,7 @@
       </c>
       <c r="R179" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty']</t>
+          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 45']</t>
         </is>
       </c>
     </row>
@@ -9633,7 +9633,7 @@
       </c>
       <c r="R180" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty']</t>
+          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 45']</t>
         </is>
       </c>
     </row>
@@ -9680,7 +9680,7 @@
       </c>
       <c r="R181" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty']</t>
+          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 45']</t>
         </is>
       </c>
     </row>
@@ -9727,7 +9727,7 @@
       </c>
       <c r="R182" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty']</t>
+          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 45']</t>
         </is>
       </c>
     </row>
@@ -9767,7 +9767,7 @@
       </c>
       <c r="R183" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty']</t>
+          <t>['Manufacturer not found', 'SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 46']</t>
         </is>
       </c>
     </row>
@@ -9808,7 +9808,7 @@
       </c>
       <c r="R184" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty']</t>
+          <t>['Manufacturer not found', 'SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 46']</t>
         </is>
       </c>
     </row>
@@ -9849,7 +9849,7 @@
       </c>
       <c r="R185" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty']</t>
+          <t>['Manufacturer not found', 'SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 46']</t>
         </is>
       </c>
     </row>
@@ -9896,7 +9896,7 @@
       </c>
       <c r="R186" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty']</t>
+          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 47']</t>
         </is>
       </c>
     </row>
@@ -9944,7 +9944,7 @@
       </c>
       <c r="R187" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty']</t>
+          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 47']</t>
         </is>
       </c>
     </row>
@@ -9992,7 +9992,7 @@
       </c>
       <c r="R188" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty']</t>
+          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 47']</t>
         </is>
       </c>
     </row>
@@ -10039,7 +10039,7 @@
       </c>
       <c r="R189" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty']</t>
+          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 48']</t>
         </is>
       </c>
     </row>
@@ -10087,7 +10087,7 @@
       </c>
       <c r="R190" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty']</t>
+          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 48']</t>
         </is>
       </c>
     </row>
@@ -10135,7 +10135,7 @@
       </c>
       <c r="R191" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty']</t>
+          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 48']</t>
         </is>
       </c>
     </row>
@@ -10182,7 +10182,7 @@
       </c>
       <c r="R192" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty']</t>
+          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 49']</t>
         </is>
       </c>
     </row>
@@ -10230,7 +10230,7 @@
       </c>
       <c r="R193" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty']</t>
+          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 49']</t>
         </is>
       </c>
     </row>
@@ -10277,7 +10277,7 @@
       </c>
       <c r="R194" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty']</t>
+          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 49']</t>
         </is>
       </c>
     </row>
@@ -10324,7 +10324,7 @@
       </c>
       <c r="R195" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty']</t>
+          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 50']</t>
         </is>
       </c>
     </row>
@@ -10371,7 +10371,7 @@
       </c>
       <c r="R196" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty']</t>
+          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 50']</t>
         </is>
       </c>
     </row>
@@ -10419,7 +10419,7 @@
       </c>
       <c r="R197" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty']</t>
+          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 50']</t>
         </is>
       </c>
     </row>
@@ -10466,7 +10466,7 @@
       </c>
       <c r="R198" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty']</t>
+          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 50']</t>
         </is>
       </c>
     </row>
@@ -10514,7 +10514,7 @@
       </c>
       <c r="R199" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty']</t>
+          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 50']</t>
         </is>
       </c>
     </row>
@@ -10561,7 +10561,7 @@
       </c>
       <c r="R200" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty']</t>
+          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 50']</t>
         </is>
       </c>
     </row>
@@ -10609,7 +10609,7 @@
       </c>
       <c r="R201" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty']</t>
+          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 50']</t>
         </is>
       </c>
     </row>
@@ -10656,7 +10656,7 @@
       </c>
       <c r="R202" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty']</t>
+          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 51']</t>
         </is>
       </c>
     </row>
@@ -10703,7 +10703,7 @@
       </c>
       <c r="R203" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty']</t>
+          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 51']</t>
         </is>
       </c>
     </row>
@@ -10751,7 +10751,7 @@
       </c>
       <c r="R204" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty']</t>
+          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 51']</t>
         </is>
       </c>
     </row>
@@ -10798,7 +10798,7 @@
       </c>
       <c r="R205" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty']</t>
+          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 51']</t>
         </is>
       </c>
     </row>
@@ -10846,7 +10846,7 @@
       </c>
       <c r="R206" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty']</t>
+          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 51']</t>
         </is>
       </c>
     </row>
@@ -10893,7 +10893,7 @@
       </c>
       <c r="R207" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty']</t>
+          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 51']</t>
         </is>
       </c>
     </row>
@@ -10941,7 +10941,7 @@
       </c>
       <c r="R208" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty']</t>
+          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 51']</t>
         </is>
       </c>
     </row>
@@ -10988,7 +10988,7 @@
       </c>
       <c r="R209" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty']</t>
+          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 52']</t>
         </is>
       </c>
     </row>
@@ -11036,7 +11036,7 @@
       </c>
       <c r="R210" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty']</t>
+          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 52']</t>
         </is>
       </c>
     </row>
@@ -11084,7 +11084,7 @@
       </c>
       <c r="R211" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty']</t>
+          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 52']</t>
         </is>
       </c>
     </row>
@@ -11131,7 +11131,7 @@
       </c>
       <c r="R212" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty']</t>
+          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 52']</t>
         </is>
       </c>
     </row>
@@ -11179,7 +11179,7 @@
       </c>
       <c r="R213" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'Model not found']</t>
+          <t>['Manufacturer not found', 'Model not found', 'page no: 53']</t>
         </is>
       </c>
     </row>
@@ -11227,7 +11227,7 @@
       </c>
       <c r="R214" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'Model not found']</t>
+          <t>['Manufacturer not found', 'Model not found', 'page no: 53']</t>
         </is>
       </c>
     </row>
@@ -11275,7 +11275,7 @@
       </c>
       <c r="R215" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'Model not found']</t>
+          <t>['Manufacturer not found', 'Model not found', 'page no: 53']</t>
         </is>
       </c>
     </row>
@@ -11323,7 +11323,7 @@
       </c>
       <c r="R216" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'Model not found']</t>
+          <t>['Manufacturer not found', 'Model not found', 'page no: 53']</t>
         </is>
       </c>
     </row>
@@ -11371,7 +11371,7 @@
       </c>
       <c r="R217" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'Model not found']</t>
+          <t>['Manufacturer not found', 'Model not found', 'page no: 53']</t>
         </is>
       </c>
     </row>
@@ -11419,7 +11419,7 @@
       </c>
       <c r="R218" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'Model not found']</t>
+          <t>['Manufacturer not found', 'Model not found', 'page no: 53']</t>
         </is>
       </c>
     </row>
@@ -11467,7 +11467,7 @@
       </c>
       <c r="R219" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'Model not found']</t>
+          <t>['Manufacturer not found', 'Model not found', 'page no: 53']</t>
         </is>
       </c>
     </row>
@@ -11515,7 +11515,7 @@
       </c>
       <c r="R220" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'Model not found']</t>
+          <t>['Manufacturer not found', 'Model not found', 'page no: 53']</t>
         </is>
       </c>
     </row>
@@ -11563,7 +11563,7 @@
       </c>
       <c r="R221" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'Model not found']</t>
+          <t>['Manufacturer not found', 'Model not found', 'page no: 53']</t>
         </is>
       </c>
     </row>
@@ -11611,7 +11611,7 @@
       </c>
       <c r="R222" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'Model not found']</t>
+          <t>['Manufacturer not found', 'Model not found', 'page no: 53']</t>
         </is>
       </c>
     </row>
@@ -11659,7 +11659,7 @@
       </c>
       <c r="R223" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'Model not found']</t>
+          <t>['Manufacturer not found', 'Model not found', 'page no: 53']</t>
         </is>
       </c>
     </row>
@@ -11707,7 +11707,7 @@
       </c>
       <c r="R224" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'Model not found']</t>
+          <t>['Manufacturer not found', 'Model not found', 'page no: 53']</t>
         </is>
       </c>
     </row>
@@ -11755,7 +11755,7 @@
       </c>
       <c r="R225" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'Model not found']</t>
+          <t>['Manufacturer not found', 'Model not found', 'page no: 53']</t>
         </is>
       </c>
     </row>
@@ -11803,7 +11803,7 @@
       </c>
       <c r="R226" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'Model not found']</t>
+          <t>['Manufacturer not found', 'Model not found', 'page no: 53']</t>
         </is>
       </c>
     </row>
@@ -11851,7 +11851,7 @@
       </c>
       <c r="R227" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'Model not found']</t>
+          <t>['Manufacturer not found', 'Model not found', 'page no: 53']</t>
         </is>
       </c>
     </row>
@@ -11899,7 +11899,7 @@
       </c>
       <c r="R228" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'Model not found']</t>
+          <t>['Manufacturer not found', 'Model not found', 'page no: 53']</t>
         </is>
       </c>
     </row>
@@ -11947,7 +11947,7 @@
       </c>
       <c r="R229" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'Model not found']</t>
+          <t>['Manufacturer not found', 'Model not found', 'page no: 53']</t>
         </is>
       </c>
     </row>
@@ -11995,7 +11995,7 @@
       </c>
       <c r="R230" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'Model not found']</t>
+          <t>['Manufacturer not found', 'Model not found', 'page no: 53']</t>
         </is>
       </c>
     </row>
@@ -12043,7 +12043,7 @@
       </c>
       <c r="R231" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'Model not found']</t>
+          <t>['Manufacturer not found', 'Model not found', 'page no: 53']</t>
         </is>
       </c>
     </row>
@@ -12091,7 +12091,7 @@
       </c>
       <c r="R232" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'Model not found']</t>
+          <t>['Manufacturer not found', 'Model not found', 'page no: 53']</t>
         </is>
       </c>
     </row>
@@ -12139,7 +12139,7 @@
       </c>
       <c r="R233" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'Model not found']</t>
+          <t>['Manufacturer not found', 'Model not found', 'page no: 54']</t>
         </is>
       </c>
     </row>
@@ -12187,7 +12187,7 @@
       </c>
       <c r="R234" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'Model not found']</t>
+          <t>['Manufacturer not found', 'Model not found', 'page no: 54']</t>
         </is>
       </c>
     </row>
@@ -12235,7 +12235,7 @@
       </c>
       <c r="R235" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'Model not found']</t>
+          <t>['Manufacturer not found', 'Model not found', 'page no: 55']</t>
         </is>
       </c>
     </row>
@@ -12283,7 +12283,7 @@
       </c>
       <c r="R236" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'Model not found']</t>
+          <t>['Manufacturer not found', 'Model not found', 'page no: 55']</t>
         </is>
       </c>
     </row>
@@ -12331,7 +12331,7 @@
       </c>
       <c r="R237" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'Model not found']</t>
+          <t>['Manufacturer not found', 'Model not found', 'page no: 56']</t>
         </is>
       </c>
     </row>
@@ -12379,7 +12379,7 @@
       </c>
       <c r="R238" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'Model not found']</t>
+          <t>['Manufacturer not found', 'Model not found', 'page no: 56']</t>
         </is>
       </c>
     </row>
@@ -12432,7 +12432,7 @@
       </c>
       <c r="R239" t="inlineStr">
         <is>
-          <t>['Manufacturer not found']</t>
+          <t>['Manufacturer not found', 'page no: 57']</t>
         </is>
       </c>
     </row>
@@ -12485,7 +12485,7 @@
       </c>
       <c r="R240" t="inlineStr">
         <is>
-          <t>['Manufacturer not found']</t>
+          <t>['Manufacturer not found', 'page no: 57']</t>
         </is>
       </c>
     </row>
@@ -12538,7 +12538,7 @@
       </c>
       <c r="R241" t="inlineStr">
         <is>
-          <t>['Manufacturer not found']</t>
+          <t>['Manufacturer not found', 'page no: 57']</t>
         </is>
       </c>
     </row>
@@ -12591,7 +12591,7 @@
       </c>
       <c r="R242" t="inlineStr">
         <is>
-          <t>['Manufacturer not found']</t>
+          <t>['Manufacturer not found', 'page no: 57']</t>
         </is>
       </c>
     </row>
@@ -12644,7 +12644,7 @@
       </c>
       <c r="R243" t="inlineStr">
         <is>
-          <t>['Manufacturer not found']</t>
+          <t>['Manufacturer not found', 'page no: 57']</t>
         </is>
       </c>
     </row>
@@ -12697,7 +12697,7 @@
       </c>
       <c r="R244" t="inlineStr">
         <is>
-          <t>['Manufacturer not found']</t>
+          <t>['Manufacturer not found', 'page no: 57']</t>
         </is>
       </c>
     </row>
@@ -12750,7 +12750,7 @@
       </c>
       <c r="R245" t="inlineStr">
         <is>
-          <t>['Manufacturer not found']</t>
+          <t>['Manufacturer not found', 'page no: 57']</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
minor bug fixes in sparrow excel processing
</commit_message>
<xml_diff>
--- a/database/Sparrows.xlsx
+++ b/database/Sparrows.xlsx
@@ -1011,6 +1011,11 @@
         </is>
       </c>
       <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>Tirfor</t>
+        </is>
+      </c>
       <c r="J11" t="inlineStr">
         <is>
           <t>SB343982</t>
@@ -1029,11 +1034,6 @@
       <c r="Q11" t="inlineStr">
         <is>
           <t>LOFT-SJB110523</t>
-        </is>
-      </c>
-      <c r="R11" t="inlineStr">
-        <is>
-          <t>['Manufacturer not found', 'page no: 8']</t>
         </is>
       </c>
     </row>
@@ -1081,7 +1081,7 @@
       </c>
       <c r="R12" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'Model not found', 'page no: 9']</t>
+          <t>['Manufacturer not found', 'Model not found', 'page no: 10']</t>
         </is>
       </c>
     </row>
@@ -1129,7 +1129,7 @@
       </c>
       <c r="R13" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'Model not found', 'page no: 10']</t>
+          <t>['Manufacturer not found', 'Model not found', 'page no: 11']</t>
         </is>
       </c>
     </row>
@@ -1879,7 +1879,7 @@
       </c>
       <c r="R27" t="inlineStr">
         <is>
-          <t>['Model not found', 'page no: 24']</t>
+          <t>['Model not found', 'page no: 25']</t>
         </is>
       </c>
     </row>
@@ -1936,7 +1936,7 @@
       </c>
       <c r="R28" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'page no: 25']</t>
+          <t>['Manufacturer not found', 'page no: 26']</t>
         </is>
       </c>
     </row>
@@ -2094,7 +2094,7 @@
       </c>
       <c r="R31" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'Model not found', 'page no: 28']</t>
+          <t>['Manufacturer not found', 'Model not found', 'page no: 29']</t>
         </is>
       </c>
     </row>
@@ -2147,7 +2147,7 @@
       </c>
       <c r="R32" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'page no: 29']</t>
+          <t>['Manufacturer not found', 'page no: 30']</t>
         </is>
       </c>
     </row>
@@ -2200,7 +2200,7 @@
       </c>
       <c r="R33" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'page no: 29']</t>
+          <t>['Manufacturer not found', 'page no: 30']</t>
         </is>
       </c>
     </row>
@@ -2253,7 +2253,7 @@
       </c>
       <c r="R34" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'page no: 29']</t>
+          <t>['Manufacturer not found', 'page no: 30']</t>
         </is>
       </c>
     </row>
@@ -2306,7 +2306,7 @@
       </c>
       <c r="R35" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'page no: 29']</t>
+          <t>['Manufacturer not found', 'page no: 30']</t>
         </is>
       </c>
     </row>
@@ -2359,7 +2359,7 @@
       </c>
       <c r="R36" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'page no: 29']</t>
+          <t>['Manufacturer not found', 'page no: 30']</t>
         </is>
       </c>
     </row>
@@ -2412,7 +2412,7 @@
       </c>
       <c r="R37" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'page no: 29']</t>
+          <t>['Manufacturer not found', 'page no: 30']</t>
         </is>
       </c>
     </row>
@@ -2465,7 +2465,7 @@
       </c>
       <c r="R38" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'page no: 30']</t>
+          <t>['Manufacturer not found', 'page no: 31']</t>
         </is>
       </c>
     </row>
@@ -2518,7 +2518,7 @@
       </c>
       <c r="R39" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'page no: 30']</t>
+          <t>['Manufacturer not found', 'page no: 31']</t>
         </is>
       </c>
     </row>
@@ -2572,7 +2572,7 @@
       </c>
       <c r="R40" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'page no: 30']</t>
+          <t>['Manufacturer not found', 'page no: 31']</t>
         </is>
       </c>
     </row>
@@ -2625,7 +2625,7 @@
       </c>
       <c r="R41" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'page no: 30']</t>
+          <t>['Manufacturer not found', 'page no: 31']</t>
         </is>
       </c>
     </row>
@@ -2678,7 +2678,7 @@
       </c>
       <c r="R42" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'page no: 30']</t>
+          <t>['Manufacturer not found', 'page no: 31']</t>
         </is>
       </c>
     </row>
@@ -2731,7 +2731,7 @@
       </c>
       <c r="R43" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'page no: 30']</t>
+          <t>['Manufacturer not found', 'page no: 31']</t>
         </is>
       </c>
     </row>
@@ -2784,7 +2784,7 @@
       </c>
       <c r="R44" t="inlineStr">
         <is>
-          <t>['Model not found', 'page no: 31']</t>
+          <t>['Model not found', 'page no: 32']</t>
         </is>
       </c>
     </row>
@@ -2837,7 +2837,7 @@
       </c>
       <c r="R45" t="inlineStr">
         <is>
-          <t>['Model not found', 'page no: 31']</t>
+          <t>['Model not found', 'page no: 32']</t>
         </is>
       </c>
     </row>
@@ -2890,7 +2890,7 @@
       </c>
       <c r="R46" t="inlineStr">
         <is>
-          <t>['Model not found', 'page no: 32']</t>
+          <t>['Model not found', 'page no: 33']</t>
         </is>
       </c>
     </row>
@@ -2943,7 +2943,7 @@
       </c>
       <c r="R47" t="inlineStr">
         <is>
-          <t>['Model not found', 'page no: 32']</t>
+          <t>['Model not found', 'page no: 33']</t>
         </is>
       </c>
     </row>
@@ -2996,7 +2996,7 @@
       </c>
       <c r="R48" t="inlineStr">
         <is>
-          <t>['Model not found', 'page no: 32']</t>
+          <t>['Model not found', 'page no: 33']</t>
         </is>
       </c>
     </row>
@@ -3049,7 +3049,7 @@
       </c>
       <c r="R49" t="inlineStr">
         <is>
-          <t>['Model not found', 'page no: 32']</t>
+          <t>['Model not found', 'page no: 33']</t>
         </is>
       </c>
     </row>
@@ -3102,7 +3102,7 @@
       </c>
       <c r="R50" t="inlineStr">
         <is>
-          <t>['Model not found', 'page no: 32']</t>
+          <t>['Model not found', 'page no: 33']</t>
         </is>
       </c>
     </row>
@@ -3155,7 +3155,7 @@
       </c>
       <c r="R51" t="inlineStr">
         <is>
-          <t>['Model not found', 'page no: 32']</t>
+          <t>['Model not found', 'page no: 33']</t>
         </is>
       </c>
     </row>
@@ -3208,7 +3208,7 @@
       </c>
       <c r="R52" t="inlineStr">
         <is>
-          <t>['Model not found', 'page no: 32']</t>
+          <t>['Model not found', 'page no: 33']</t>
         </is>
       </c>
     </row>
@@ -3261,7 +3261,7 @@
       </c>
       <c r="R53" t="inlineStr">
         <is>
-          <t>['Model not found', 'page no: 32']</t>
+          <t>['Model not found', 'page no: 33']</t>
         </is>
       </c>
     </row>
@@ -3314,7 +3314,7 @@
       </c>
       <c r="R54" t="inlineStr">
         <is>
-          <t>['Model not found', 'page no: 32']</t>
+          <t>['Model not found', 'page no: 33']</t>
         </is>
       </c>
     </row>
@@ -3367,7 +3367,7 @@
       </c>
       <c r="R55" t="inlineStr">
         <is>
-          <t>['Model not found', 'page no: 32']</t>
+          <t>['Model not found', 'page no: 33']</t>
         </is>
       </c>
     </row>
@@ -3420,7 +3420,7 @@
       </c>
       <c r="R56" t="inlineStr">
         <is>
-          <t>['Model not found', 'page no: 32']</t>
+          <t>['Model not found', 'page no: 33']</t>
         </is>
       </c>
     </row>
@@ -3473,7 +3473,7 @@
       </c>
       <c r="R57" t="inlineStr">
         <is>
-          <t>['Model not found', 'page no: 32']</t>
+          <t>['Model not found', 'page no: 33']</t>
         </is>
       </c>
     </row>
@@ -3526,7 +3526,7 @@
       </c>
       <c r="R58" t="inlineStr">
         <is>
-          <t>['Model not found', 'page no: 33']</t>
+          <t>['Model not found', 'page no: 34']</t>
         </is>
       </c>
     </row>
@@ -3579,7 +3579,7 @@
       </c>
       <c r="R59" t="inlineStr">
         <is>
-          <t>['Model not found', 'page no: 33']</t>
+          <t>['Model not found', 'page no: 34']</t>
         </is>
       </c>
     </row>
@@ -3632,7 +3632,7 @@
       </c>
       <c r="R60" t="inlineStr">
         <is>
-          <t>['Model not found', 'page no: 33']</t>
+          <t>['Model not found', 'page no: 34']</t>
         </is>
       </c>
     </row>
@@ -3685,7 +3685,7 @@
       </c>
       <c r="R61" t="inlineStr">
         <is>
-          <t>['Model not found', 'page no: 33']</t>
+          <t>['Model not found', 'page no: 34']</t>
         </is>
       </c>
     </row>
@@ -3738,7 +3738,7 @@
       </c>
       <c r="R62" t="inlineStr">
         <is>
-          <t>['Model not found', 'page no: 33']</t>
+          <t>['Model not found', 'page no: 34']</t>
         </is>
       </c>
     </row>
@@ -3791,7 +3791,7 @@
       </c>
       <c r="R63" t="inlineStr">
         <is>
-          <t>['Model not found', 'page no: 33']</t>
+          <t>['Model not found', 'page no: 34']</t>
         </is>
       </c>
     </row>
@@ -3844,7 +3844,7 @@
       </c>
       <c r="R64" t="inlineStr">
         <is>
-          <t>['Model not found', 'page no: 33']</t>
+          <t>['Model not found', 'page no: 34']</t>
         </is>
       </c>
     </row>
@@ -3897,7 +3897,7 @@
       </c>
       <c r="R65" t="inlineStr">
         <is>
-          <t>['Model not found', 'page no: 33']</t>
+          <t>['Model not found', 'page no: 34']</t>
         </is>
       </c>
     </row>
@@ -3950,7 +3950,7 @@
       </c>
       <c r="R66" t="inlineStr">
         <is>
-          <t>['Model not found', 'page no: 34']</t>
+          <t>['Model not found', 'page no: 35']</t>
         </is>
       </c>
     </row>
@@ -4003,7 +4003,7 @@
       </c>
       <c r="R67" t="inlineStr">
         <is>
-          <t>['Model not found', 'page no: 34']</t>
+          <t>['Model not found', 'page no: 35']</t>
         </is>
       </c>
     </row>
@@ -4056,7 +4056,7 @@
       </c>
       <c r="R68" t="inlineStr">
         <is>
-          <t>['Model not found', 'page no: 34']</t>
+          <t>['Model not found', 'page no: 35']</t>
         </is>
       </c>
     </row>
@@ -4109,7 +4109,7 @@
       </c>
       <c r="R69" t="inlineStr">
         <is>
-          <t>['Model not found', 'page no: 34']</t>
+          <t>['Model not found', 'page no: 35']</t>
         </is>
       </c>
     </row>
@@ -4140,6 +4140,11 @@
         </is>
       </c>
       <c r="H70" t="inlineStr"/>
+      <c r="I70" t="inlineStr">
+        <is>
+          <t>Van Beest</t>
+        </is>
+      </c>
       <c r="J70" t="inlineStr">
         <is>
           <t>SB344075</t>
@@ -4158,11 +4163,6 @@
       <c r="Q70" t="inlineStr">
         <is>
           <t>LOFT-SJB110523</t>
-        </is>
-      </c>
-      <c r="R70" t="inlineStr">
-        <is>
-          <t>['Manufacturer not found', 'page no: 35']</t>
         </is>
       </c>
     </row>
@@ -4193,6 +4193,11 @@
         </is>
       </c>
       <c r="H71" t="inlineStr"/>
+      <c r="I71" t="inlineStr">
+        <is>
+          <t>Van Beest</t>
+        </is>
+      </c>
       <c r="J71" t="inlineStr">
         <is>
           <t>SB344075</t>
@@ -4211,11 +4216,6 @@
       <c r="Q71" t="inlineStr">
         <is>
           <t>LOFT-SJB110523</t>
-        </is>
-      </c>
-      <c r="R71" t="inlineStr">
-        <is>
-          <t>['Manufacturer not found', 'page no: 35']</t>
         </is>
       </c>
     </row>
@@ -4246,6 +4246,11 @@
         </is>
       </c>
       <c r="H72" t="inlineStr"/>
+      <c r="I72" t="inlineStr">
+        <is>
+          <t>Van Beest</t>
+        </is>
+      </c>
       <c r="J72" t="inlineStr">
         <is>
           <t>SB344075</t>
@@ -4264,11 +4269,6 @@
       <c r="Q72" t="inlineStr">
         <is>
           <t>LOFT-SJB110523</t>
-        </is>
-      </c>
-      <c r="R72" t="inlineStr">
-        <is>
-          <t>['Manufacturer not found', 'page no: 35']</t>
         </is>
       </c>
     </row>
@@ -4299,6 +4299,11 @@
         </is>
       </c>
       <c r="H73" t="inlineStr"/>
+      <c r="I73" t="inlineStr">
+        <is>
+          <t>Van Beest</t>
+        </is>
+      </c>
       <c r="J73" t="inlineStr">
         <is>
           <t>SB344075</t>
@@ -4317,11 +4322,6 @@
       <c r="Q73" t="inlineStr">
         <is>
           <t>LOFT-SJB110523</t>
-        </is>
-      </c>
-      <c r="R73" t="inlineStr">
-        <is>
-          <t>['Manufacturer not found', 'page no: 35']</t>
         </is>
       </c>
     </row>
@@ -4352,6 +4352,11 @@
         </is>
       </c>
       <c r="H74" t="inlineStr"/>
+      <c r="I74" t="inlineStr">
+        <is>
+          <t>Van Beest</t>
+        </is>
+      </c>
       <c r="J74" t="inlineStr">
         <is>
           <t>SB344075</t>
@@ -4370,11 +4375,6 @@
       <c r="Q74" t="inlineStr">
         <is>
           <t>LOFT-SJB110523</t>
-        </is>
-      </c>
-      <c r="R74" t="inlineStr">
-        <is>
-          <t>['Manufacturer not found', 'page no: 35']</t>
         </is>
       </c>
     </row>
@@ -4405,6 +4405,11 @@
         </is>
       </c>
       <c r="H75" t="inlineStr"/>
+      <c r="I75" t="inlineStr">
+        <is>
+          <t>Van Beest</t>
+        </is>
+      </c>
       <c r="J75" t="inlineStr">
         <is>
           <t>SB344075</t>
@@ -4423,11 +4428,6 @@
       <c r="Q75" t="inlineStr">
         <is>
           <t>LOFT-SJB110523</t>
-        </is>
-      </c>
-      <c r="R75" t="inlineStr">
-        <is>
-          <t>['Manufacturer not found', 'page no: 35']</t>
         </is>
       </c>
     </row>
@@ -4458,6 +4458,11 @@
         </is>
       </c>
       <c r="H76" t="inlineStr"/>
+      <c r="I76" t="inlineStr">
+        <is>
+          <t>Van Beest</t>
+        </is>
+      </c>
       <c r="J76" t="inlineStr">
         <is>
           <t>SB344075</t>
@@ -4476,11 +4481,6 @@
       <c r="Q76" t="inlineStr">
         <is>
           <t>LOFT-SJB110523</t>
-        </is>
-      </c>
-      <c r="R76" t="inlineStr">
-        <is>
-          <t>['Manufacturer not found', 'page no: 35']</t>
         </is>
       </c>
     </row>
@@ -4511,6 +4511,11 @@
         </is>
       </c>
       <c r="H77" t="inlineStr"/>
+      <c r="I77" t="inlineStr">
+        <is>
+          <t>Van Beest</t>
+        </is>
+      </c>
       <c r="J77" t="inlineStr">
         <is>
           <t>SB344075</t>
@@ -4529,11 +4534,6 @@
       <c r="Q77" t="inlineStr">
         <is>
           <t>LOFT-SJB110523</t>
-        </is>
-      </c>
-      <c r="R77" t="inlineStr">
-        <is>
-          <t>['Manufacturer not found', 'page no: 35']</t>
         </is>
       </c>
     </row>
@@ -4564,6 +4564,11 @@
         </is>
       </c>
       <c r="H78" t="inlineStr"/>
+      <c r="I78" t="inlineStr">
+        <is>
+          <t>Van Beest</t>
+        </is>
+      </c>
       <c r="J78" t="inlineStr">
         <is>
           <t>SB344075</t>
@@ -4582,11 +4587,6 @@
       <c r="Q78" t="inlineStr">
         <is>
           <t>LOFT-SJB110523</t>
-        </is>
-      </c>
-      <c r="R78" t="inlineStr">
-        <is>
-          <t>['Manufacturer not found', 'page no: 35']</t>
         </is>
       </c>
     </row>
@@ -4617,6 +4617,11 @@
         </is>
       </c>
       <c r="H79" t="inlineStr"/>
+      <c r="I79" t="inlineStr">
+        <is>
+          <t>Van Beest</t>
+        </is>
+      </c>
       <c r="J79" t="inlineStr">
         <is>
           <t>SB344075</t>
@@ -4635,11 +4640,6 @@
       <c r="Q79" t="inlineStr">
         <is>
           <t>LOFT-SJB110523</t>
-        </is>
-      </c>
-      <c r="R79" t="inlineStr">
-        <is>
-          <t>['Manufacturer not found', 'page no: 35']</t>
         </is>
       </c>
     </row>
@@ -4670,6 +4670,11 @@
         </is>
       </c>
       <c r="H80" t="inlineStr"/>
+      <c r="I80" t="inlineStr">
+        <is>
+          <t>Van Beest</t>
+        </is>
+      </c>
       <c r="J80" t="inlineStr">
         <is>
           <t>SB344075</t>
@@ -4688,11 +4693,6 @@
       <c r="Q80" t="inlineStr">
         <is>
           <t>LOFT-SJB110523</t>
-        </is>
-      </c>
-      <c r="R80" t="inlineStr">
-        <is>
-          <t>['Manufacturer not found', 'page no: 35']</t>
         </is>
       </c>
     </row>
@@ -4723,6 +4723,11 @@
         </is>
       </c>
       <c r="H81" t="inlineStr"/>
+      <c r="I81" t="inlineStr">
+        <is>
+          <t>Van Beest</t>
+        </is>
+      </c>
       <c r="J81" t="inlineStr">
         <is>
           <t>SB344075</t>
@@ -4741,11 +4746,6 @@
       <c r="Q81" t="inlineStr">
         <is>
           <t>LOFT-SJB110523</t>
-        </is>
-      </c>
-      <c r="R81" t="inlineStr">
-        <is>
-          <t>['Manufacturer not found', 'page no: 35']</t>
         </is>
       </c>
     </row>
@@ -4776,6 +4776,11 @@
         </is>
       </c>
       <c r="H82" t="inlineStr"/>
+      <c r="I82" t="inlineStr">
+        <is>
+          <t>Van Beest</t>
+        </is>
+      </c>
       <c r="J82" t="inlineStr">
         <is>
           <t>SB344075</t>
@@ -4794,11 +4799,6 @@
       <c r="Q82" t="inlineStr">
         <is>
           <t>LOFT-SJB110523</t>
-        </is>
-      </c>
-      <c r="R82" t="inlineStr">
-        <is>
-          <t>['Manufacturer not found', 'page no: 35']</t>
         </is>
       </c>
     </row>
@@ -4829,6 +4829,11 @@
         </is>
       </c>
       <c r="H83" t="inlineStr"/>
+      <c r="I83" t="inlineStr">
+        <is>
+          <t>Van Beest</t>
+        </is>
+      </c>
       <c r="J83" t="inlineStr">
         <is>
           <t>SB344075</t>
@@ -4847,11 +4852,6 @@
       <c r="Q83" t="inlineStr">
         <is>
           <t>LOFT-SJB110523</t>
-        </is>
-      </c>
-      <c r="R83" t="inlineStr">
-        <is>
-          <t>['Manufacturer not found', 'page no: 35']</t>
         </is>
       </c>
     </row>
@@ -4882,6 +4882,11 @@
         </is>
       </c>
       <c r="H84" t="inlineStr"/>
+      <c r="I84" t="inlineStr">
+        <is>
+          <t>Van Beest</t>
+        </is>
+      </c>
       <c r="J84" t="inlineStr">
         <is>
           <t>SB344075</t>
@@ -4900,11 +4905,6 @@
       <c r="Q84" t="inlineStr">
         <is>
           <t>LOFT-SJB110523</t>
-        </is>
-      </c>
-      <c r="R84" t="inlineStr">
-        <is>
-          <t>['Manufacturer not found', 'page no: 35']</t>
         </is>
       </c>
     </row>
@@ -4935,6 +4935,11 @@
         </is>
       </c>
       <c r="H85" t="inlineStr"/>
+      <c r="I85" t="inlineStr">
+        <is>
+          <t>Van Beest</t>
+        </is>
+      </c>
       <c r="J85" t="inlineStr">
         <is>
           <t>SB344075</t>
@@ -4953,11 +4958,6 @@
       <c r="Q85" t="inlineStr">
         <is>
           <t>LOFT-SJB110523</t>
-        </is>
-      </c>
-      <c r="R85" t="inlineStr">
-        <is>
-          <t>['Manufacturer not found', 'page no: 35']</t>
         </is>
       </c>
     </row>
@@ -4988,6 +4988,11 @@
         </is>
       </c>
       <c r="H86" t="inlineStr"/>
+      <c r="I86" t="inlineStr">
+        <is>
+          <t>Van Beest</t>
+        </is>
+      </c>
       <c r="J86" t="inlineStr">
         <is>
           <t>SB344075</t>
@@ -5006,11 +5011,6 @@
       <c r="Q86" t="inlineStr">
         <is>
           <t>LOFT-SJB110523</t>
-        </is>
-      </c>
-      <c r="R86" t="inlineStr">
-        <is>
-          <t>['Manufacturer not found', 'page no: 35']</t>
         </is>
       </c>
     </row>
@@ -5041,6 +5041,11 @@
         </is>
       </c>
       <c r="H87" t="inlineStr"/>
+      <c r="I87" t="inlineStr">
+        <is>
+          <t>Van Beest</t>
+        </is>
+      </c>
       <c r="J87" t="inlineStr">
         <is>
           <t>SB344075</t>
@@ -5059,11 +5064,6 @@
       <c r="Q87" t="inlineStr">
         <is>
           <t>LOFT-SJB110523</t>
-        </is>
-      </c>
-      <c r="R87" t="inlineStr">
-        <is>
-          <t>['Manufacturer not found', 'page no: 35']</t>
         </is>
       </c>
     </row>
@@ -5094,6 +5094,11 @@
         </is>
       </c>
       <c r="H88" t="inlineStr"/>
+      <c r="I88" t="inlineStr">
+        <is>
+          <t>Van Beest</t>
+        </is>
+      </c>
       <c r="J88" t="inlineStr">
         <is>
           <t>SB344075</t>
@@ -5112,11 +5117,6 @@
       <c r="Q88" t="inlineStr">
         <is>
           <t>LOFT-SJB110523</t>
-        </is>
-      </c>
-      <c r="R88" t="inlineStr">
-        <is>
-          <t>['Manufacturer not found', 'page no: 35']</t>
         </is>
       </c>
     </row>
@@ -5147,6 +5147,11 @@
         </is>
       </c>
       <c r="H89" t="inlineStr"/>
+      <c r="I89" t="inlineStr">
+        <is>
+          <t>Van Beest</t>
+        </is>
+      </c>
       <c r="J89" t="inlineStr">
         <is>
           <t>SB344075</t>
@@ -5165,11 +5170,6 @@
       <c r="Q89" t="inlineStr">
         <is>
           <t>LOFT-SJB110523</t>
-        </is>
-      </c>
-      <c r="R89" t="inlineStr">
-        <is>
-          <t>['Manufacturer not found', 'page no: 35']</t>
         </is>
       </c>
     </row>
@@ -5200,6 +5200,11 @@
         </is>
       </c>
       <c r="H90" t="inlineStr"/>
+      <c r="I90" t="inlineStr">
+        <is>
+          <t>Van Beest</t>
+        </is>
+      </c>
       <c r="J90" t="inlineStr">
         <is>
           <t>SB344075</t>
@@ -5218,11 +5223,6 @@
       <c r="Q90" t="inlineStr">
         <is>
           <t>LOFT-SJB110523</t>
-        </is>
-      </c>
-      <c r="R90" t="inlineStr">
-        <is>
-          <t>['Manufacturer not found', 'page no: 35']</t>
         </is>
       </c>
     </row>
@@ -5253,6 +5253,11 @@
         </is>
       </c>
       <c r="H91" t="inlineStr"/>
+      <c r="I91" t="inlineStr">
+        <is>
+          <t>Van Beest</t>
+        </is>
+      </c>
       <c r="J91" t="inlineStr">
         <is>
           <t>SB344075</t>
@@ -5271,11 +5276,6 @@
       <c r="Q91" t="inlineStr">
         <is>
           <t>LOFT-SJB110523</t>
-        </is>
-      </c>
-      <c r="R91" t="inlineStr">
-        <is>
-          <t>['Manufacturer not found', 'page no: 35']</t>
         </is>
       </c>
     </row>
@@ -5306,6 +5306,11 @@
         </is>
       </c>
       <c r="H92" t="inlineStr"/>
+      <c r="I92" t="inlineStr">
+        <is>
+          <t>Van Beest</t>
+        </is>
+      </c>
       <c r="J92" t="inlineStr">
         <is>
           <t>SB344075</t>
@@ -5324,11 +5329,6 @@
       <c r="Q92" t="inlineStr">
         <is>
           <t>LOFT-SJB110523</t>
-        </is>
-      </c>
-      <c r="R92" t="inlineStr">
-        <is>
-          <t>['Manufacturer not found', 'page no: 35']</t>
         </is>
       </c>
     </row>
@@ -5359,6 +5359,11 @@
         </is>
       </c>
       <c r="H93" t="inlineStr"/>
+      <c r="I93" t="inlineStr">
+        <is>
+          <t>Van Beest</t>
+        </is>
+      </c>
       <c r="J93" t="inlineStr">
         <is>
           <t>SB344075</t>
@@ -5377,11 +5382,6 @@
       <c r="Q93" t="inlineStr">
         <is>
           <t>LOFT-SJB110523</t>
-        </is>
-      </c>
-      <c r="R93" t="inlineStr">
-        <is>
-          <t>['Manufacturer not found', 'page no: 35']</t>
         </is>
       </c>
     </row>
@@ -5412,6 +5412,11 @@
         </is>
       </c>
       <c r="H94" t="inlineStr"/>
+      <c r="I94" t="inlineStr">
+        <is>
+          <t>Van Beest</t>
+        </is>
+      </c>
       <c r="J94" t="inlineStr">
         <is>
           <t>SB344075</t>
@@ -5430,11 +5435,6 @@
       <c r="Q94" t="inlineStr">
         <is>
           <t>LOFT-SJB110523</t>
-        </is>
-      </c>
-      <c r="R94" t="inlineStr">
-        <is>
-          <t>['Manufacturer not found', 'page no: 35']</t>
         </is>
       </c>
     </row>
@@ -5465,6 +5465,11 @@
         </is>
       </c>
       <c r="H95" t="inlineStr"/>
+      <c r="I95" t="inlineStr">
+        <is>
+          <t>Van Beest</t>
+        </is>
+      </c>
       <c r="J95" t="inlineStr">
         <is>
           <t>SB344075</t>
@@ -5483,11 +5488,6 @@
       <c r="Q95" t="inlineStr">
         <is>
           <t>LOFT-SJB110523</t>
-        </is>
-      </c>
-      <c r="R95" t="inlineStr">
-        <is>
-          <t>['Manufacturer not found', 'page no: 35']</t>
         </is>
       </c>
     </row>
@@ -5518,6 +5518,11 @@
         </is>
       </c>
       <c r="H96" t="inlineStr"/>
+      <c r="I96" t="inlineStr">
+        <is>
+          <t>Van Beest</t>
+        </is>
+      </c>
       <c r="J96" t="inlineStr">
         <is>
           <t>SB344075</t>
@@ -5536,11 +5541,6 @@
       <c r="Q96" t="inlineStr">
         <is>
           <t>LOFT-SJB110523</t>
-        </is>
-      </c>
-      <c r="R96" t="inlineStr">
-        <is>
-          <t>['Manufacturer not found', 'page no: 35']</t>
         </is>
       </c>
     </row>
@@ -5571,6 +5571,11 @@
         </is>
       </c>
       <c r="H97" t="inlineStr"/>
+      <c r="I97" t="inlineStr">
+        <is>
+          <t>Van Beest</t>
+        </is>
+      </c>
       <c r="J97" t="inlineStr">
         <is>
           <t>SB344075</t>
@@ -5589,11 +5594,6 @@
       <c r="Q97" t="inlineStr">
         <is>
           <t>LOFT-SJB110523</t>
-        </is>
-      </c>
-      <c r="R97" t="inlineStr">
-        <is>
-          <t>['Manufacturer not found', 'page no: 35']</t>
         </is>
       </c>
     </row>
@@ -5624,6 +5624,11 @@
         </is>
       </c>
       <c r="H98" t="inlineStr"/>
+      <c r="I98" t="inlineStr">
+        <is>
+          <t>Van Beest</t>
+        </is>
+      </c>
       <c r="J98" t="inlineStr">
         <is>
           <t>SB344075</t>
@@ -5642,11 +5647,6 @@
       <c r="Q98" t="inlineStr">
         <is>
           <t>LOFT-SJB110523</t>
-        </is>
-      </c>
-      <c r="R98" t="inlineStr">
-        <is>
-          <t>['Manufacturer not found', 'page no: 35']</t>
         </is>
       </c>
     </row>
@@ -5677,6 +5677,11 @@
         </is>
       </c>
       <c r="H99" t="inlineStr"/>
+      <c r="I99" t="inlineStr">
+        <is>
+          <t>Van Beest</t>
+        </is>
+      </c>
       <c r="J99" t="inlineStr">
         <is>
           <t>SB344075</t>
@@ -5695,11 +5700,6 @@
       <c r="Q99" t="inlineStr">
         <is>
           <t>LOFT-SJB110523</t>
-        </is>
-      </c>
-      <c r="R99" t="inlineStr">
-        <is>
-          <t>['Manufacturer not found', 'page no: 35']</t>
         </is>
       </c>
     </row>
@@ -5730,6 +5730,11 @@
         </is>
       </c>
       <c r="H100" t="inlineStr"/>
+      <c r="I100" t="inlineStr">
+        <is>
+          <t>Van Beest</t>
+        </is>
+      </c>
       <c r="J100" t="inlineStr">
         <is>
           <t>SB344075</t>
@@ -5748,11 +5753,6 @@
       <c r="Q100" t="inlineStr">
         <is>
           <t>LOFT-SJB110523</t>
-        </is>
-      </c>
-      <c r="R100" t="inlineStr">
-        <is>
-          <t>['Manufacturer not found', 'page no: 35']</t>
         </is>
       </c>
     </row>
@@ -5783,6 +5783,11 @@
         </is>
       </c>
       <c r="H101" t="inlineStr"/>
+      <c r="I101" t="inlineStr">
+        <is>
+          <t>Van Beest</t>
+        </is>
+      </c>
       <c r="J101" t="inlineStr">
         <is>
           <t>SB344075</t>
@@ -5801,11 +5806,6 @@
       <c r="Q101" t="inlineStr">
         <is>
           <t>LOFT-SJB110523</t>
-        </is>
-      </c>
-      <c r="R101" t="inlineStr">
-        <is>
-          <t>['Manufacturer not found', 'page no: 35']</t>
         </is>
       </c>
     </row>
@@ -5836,6 +5836,11 @@
         </is>
       </c>
       <c r="H102" t="inlineStr"/>
+      <c r="I102" t="inlineStr">
+        <is>
+          <t>Van Beest</t>
+        </is>
+      </c>
       <c r="J102" t="inlineStr">
         <is>
           <t>SB344075</t>
@@ -5854,11 +5859,6 @@
       <c r="Q102" t="inlineStr">
         <is>
           <t>LOFT-SJB110523</t>
-        </is>
-      </c>
-      <c r="R102" t="inlineStr">
-        <is>
-          <t>['Manufacturer not found', 'page no: 35']</t>
         </is>
       </c>
     </row>
@@ -5889,6 +5889,11 @@
         </is>
       </c>
       <c r="H103" t="inlineStr"/>
+      <c r="I103" t="inlineStr">
+        <is>
+          <t>Van Beest</t>
+        </is>
+      </c>
       <c r="J103" t="inlineStr">
         <is>
           <t>SB344075</t>
@@ -5907,11 +5912,6 @@
       <c r="Q103" t="inlineStr">
         <is>
           <t>LOFT-SJB110523</t>
-        </is>
-      </c>
-      <c r="R103" t="inlineStr">
-        <is>
-          <t>['Manufacturer not found', 'page no: 35']</t>
         </is>
       </c>
     </row>
@@ -5942,6 +5942,11 @@
         </is>
       </c>
       <c r="H104" t="inlineStr"/>
+      <c r="I104" t="inlineStr">
+        <is>
+          <t>Van Beest</t>
+        </is>
+      </c>
       <c r="J104" t="inlineStr">
         <is>
           <t>SB344075</t>
@@ -5960,11 +5965,6 @@
       <c r="Q104" t="inlineStr">
         <is>
           <t>LOFT-SJB110523</t>
-        </is>
-      </c>
-      <c r="R104" t="inlineStr">
-        <is>
-          <t>['Manufacturer not found', 'page no: 35']</t>
         </is>
       </c>
     </row>
@@ -5995,6 +5995,11 @@
         </is>
       </c>
       <c r="H105" t="inlineStr"/>
+      <c r="I105" t="inlineStr">
+        <is>
+          <t>Van Beest</t>
+        </is>
+      </c>
       <c r="J105" t="inlineStr">
         <is>
           <t>SB344075</t>
@@ -6013,11 +6018,6 @@
       <c r="Q105" t="inlineStr">
         <is>
           <t>LOFT-SJB110523</t>
-        </is>
-      </c>
-      <c r="R105" t="inlineStr">
-        <is>
-          <t>['Manufacturer not found', 'page no: 35']</t>
         </is>
       </c>
     </row>
@@ -6065,7 +6065,7 @@
       </c>
       <c r="R106" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'Model not found', 'page no: 36']</t>
+          <t>['Manufacturer not found', 'Model not found', 'page no: 37']</t>
         </is>
       </c>
     </row>
@@ -6113,7 +6113,7 @@
       </c>
       <c r="R107" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'Model not found', 'page no: 36']</t>
+          <t>['Manufacturer not found', 'Model not found', 'page no: 37']</t>
         </is>
       </c>
     </row>
@@ -6161,7 +6161,7 @@
       </c>
       <c r="R108" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'Model not found', 'page no: 36']</t>
+          <t>['Manufacturer not found', 'Model not found', 'page no: 37']</t>
         </is>
       </c>
     </row>
@@ -6209,7 +6209,7 @@
       </c>
       <c r="R109" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'Model not found', 'page no: 36']</t>
+          <t>['Manufacturer not found', 'Model not found', 'page no: 37']</t>
         </is>
       </c>
     </row>
@@ -6257,7 +6257,7 @@
       </c>
       <c r="R110" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'Model not found', 'page no: 36']</t>
+          <t>['Manufacturer not found', 'Model not found', 'page no: 37']</t>
         </is>
       </c>
     </row>
@@ -6305,7 +6305,7 @@
       </c>
       <c r="R111" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'Model not found', 'page no: 36']</t>
+          <t>['Manufacturer not found', 'Model not found', 'page no: 37']</t>
         </is>
       </c>
     </row>
@@ -6358,7 +6358,7 @@
       </c>
       <c r="R112" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'page no: 37']</t>
+          <t>['Manufacturer not found', 'page no: 38']</t>
         </is>
       </c>
     </row>
@@ -6411,7 +6411,7 @@
       </c>
       <c r="R113" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'page no: 37']</t>
+          <t>['Manufacturer not found', 'page no: 38']</t>
         </is>
       </c>
     </row>
@@ -6464,7 +6464,7 @@
       </c>
       <c r="R114" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'page no: 37']</t>
+          <t>['Manufacturer not found', 'page no: 38']</t>
         </is>
       </c>
     </row>
@@ -6517,7 +6517,7 @@
       </c>
       <c r="R115" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'page no: 37']</t>
+          <t>['Manufacturer not found', 'page no: 38']</t>
         </is>
       </c>
     </row>
@@ -6570,7 +6570,7 @@
       </c>
       <c r="R116" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'page no: 37']</t>
+          <t>['Manufacturer not found', 'page no: 38']</t>
         </is>
       </c>
     </row>
@@ -6623,7 +6623,7 @@
       </c>
       <c r="R117" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'page no: 37']</t>
+          <t>['Manufacturer not found', 'page no: 38']</t>
         </is>
       </c>
     </row>
@@ -6676,7 +6676,7 @@
       </c>
       <c r="R118" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'page no: 37']</t>
+          <t>['Manufacturer not found', 'page no: 38']</t>
         </is>
       </c>
     </row>
@@ -6729,7 +6729,7 @@
       </c>
       <c r="R119" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'page no: 37']</t>
+          <t>['Manufacturer not found', 'page no: 38']</t>
         </is>
       </c>
     </row>
@@ -6782,7 +6782,7 @@
       </c>
       <c r="R120" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'page no: 37']</t>
+          <t>['Manufacturer not found', 'page no: 38']</t>
         </is>
       </c>
     </row>
@@ -6835,7 +6835,7 @@
       </c>
       <c r="R121" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'page no: 37']</t>
+          <t>['Manufacturer not found', 'page no: 38']</t>
         </is>
       </c>
     </row>
@@ -6883,7 +6883,7 @@
       </c>
       <c r="R122" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'Model not found', 'page no: 38']</t>
+          <t>['Manufacturer not found', 'Model not found', 'page no: 39']</t>
         </is>
       </c>
     </row>
@@ -6931,7 +6931,7 @@
       </c>
       <c r="R123" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'Model not found', 'page no: 38']</t>
+          <t>['Manufacturer not found', 'Model not found', 'page no: 39']</t>
         </is>
       </c>
     </row>
@@ -6979,7 +6979,7 @@
       </c>
       <c r="R124" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'Model not found', 'page no: 38']</t>
+          <t>['Manufacturer not found', 'Model not found', 'page no: 39']</t>
         </is>
       </c>
     </row>
@@ -7027,7 +7027,7 @@
       </c>
       <c r="R125" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'Model not found', 'page no: 38']</t>
+          <t>['Manufacturer not found', 'Model not found', 'page no: 39']</t>
         </is>
       </c>
     </row>
@@ -7075,7 +7075,7 @@
       </c>
       <c r="R126" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'Model not found', 'page no: 38']</t>
+          <t>['Manufacturer not found', 'Model not found', 'page no: 39']</t>
         </is>
       </c>
     </row>
@@ -7123,7 +7123,7 @@
       </c>
       <c r="R127" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'Model not found', 'page no: 38']</t>
+          <t>['Manufacturer not found', 'Model not found', 'page no: 39']</t>
         </is>
       </c>
     </row>
@@ -7171,7 +7171,7 @@
       </c>
       <c r="R128" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'Model not found', 'page no: 39']</t>
+          <t>['Manufacturer not found', 'Model not found', 'page no: 40']</t>
         </is>
       </c>
     </row>
@@ -7219,7 +7219,7 @@
       </c>
       <c r="R129" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'Model not found', 'page no: 39']</t>
+          <t>['Manufacturer not found', 'Model not found', 'page no: 40']</t>
         </is>
       </c>
     </row>
@@ -7267,7 +7267,7 @@
       </c>
       <c r="R130" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'Model not found', 'page no: 39']</t>
+          <t>['Manufacturer not found', 'Model not found', 'page no: 40']</t>
         </is>
       </c>
     </row>
@@ -7315,7 +7315,7 @@
       </c>
       <c r="R131" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'Model not found', 'page no: 39']</t>
+          <t>['Manufacturer not found', 'Model not found', 'page no: 40']</t>
         </is>
       </c>
     </row>
@@ -7474,7 +7474,7 @@
       </c>
       <c r="R134" t="inlineStr">
         <is>
-          <t>['Model not found', 'page no: 41']</t>
+          <t>['Model not found', 'page no: 42']</t>
         </is>
       </c>
     </row>
@@ -7516,7 +7516,7 @@
       </c>
       <c r="R135" t="inlineStr">
         <is>
-          <t>['Model not found', 'SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 42']</t>
+          <t>['Model not found', 'SWL not found in the page', 'page no: 43']</t>
         </is>
       </c>
     </row>
@@ -7559,7 +7559,7 @@
       </c>
       <c r="R136" t="inlineStr">
         <is>
-          <t>['Model not found', 'SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 42']</t>
+          <t>['Model not found', 'SWL not found in the page', 'page no: 43']</t>
         </is>
       </c>
     </row>
@@ -7601,7 +7601,7 @@
       </c>
       <c r="R137" t="inlineStr">
         <is>
-          <t>['Model not found', 'SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 42']</t>
+          <t>['Model not found', 'SWL not found in the page', 'page no: 43']</t>
         </is>
       </c>
     </row>
@@ -7644,7 +7644,7 @@
       </c>
       <c r="R138" t="inlineStr">
         <is>
-          <t>['Model not found', 'SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 42']</t>
+          <t>['Model not found', 'SWL not found in the page', 'page no: 43']</t>
         </is>
       </c>
     </row>
@@ -7691,7 +7691,7 @@
       </c>
       <c r="R139" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 43']</t>
+          <t>['SWL not found in the page', 'page no: 44']</t>
         </is>
       </c>
     </row>
@@ -7738,7 +7738,7 @@
       </c>
       <c r="R140" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 43']</t>
+          <t>['SWL not found in the page', 'page no: 44']</t>
         </is>
       </c>
     </row>
@@ -7785,7 +7785,7 @@
       </c>
       <c r="R141" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 43']</t>
+          <t>['SWL not found in the page', 'page no: 44']</t>
         </is>
       </c>
     </row>
@@ -7832,7 +7832,7 @@
       </c>
       <c r="R142" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 43']</t>
+          <t>['SWL not found in the page', 'page no: 44']</t>
         </is>
       </c>
     </row>
@@ -7879,7 +7879,7 @@
       </c>
       <c r="R143" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 43']</t>
+          <t>['SWL not found in the page', 'page no: 44']</t>
         </is>
       </c>
     </row>
@@ -7926,7 +7926,7 @@
       </c>
       <c r="R144" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 43']</t>
+          <t>['SWL not found in the page', 'page no: 44']</t>
         </is>
       </c>
     </row>
@@ -7973,7 +7973,7 @@
       </c>
       <c r="R145" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 43']</t>
+          <t>['SWL not found in the page', 'page no: 44']</t>
         </is>
       </c>
     </row>
@@ -8020,7 +8020,7 @@
       </c>
       <c r="R146" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 43']</t>
+          <t>['SWL not found in the page', 'page no: 44']</t>
         </is>
       </c>
     </row>
@@ -8067,7 +8067,7 @@
       </c>
       <c r="R147" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 43']</t>
+          <t>['SWL not found in the page', 'page no: 44']</t>
         </is>
       </c>
     </row>
@@ -8114,7 +8114,7 @@
       </c>
       <c r="R148" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 43']</t>
+          <t>['SWL not found in the page', 'page no: 44']</t>
         </is>
       </c>
     </row>
@@ -8161,7 +8161,7 @@
       </c>
       <c r="R149" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 43']</t>
+          <t>['SWL not found in the page', 'page no: 44']</t>
         </is>
       </c>
     </row>
@@ -8208,7 +8208,7 @@
       </c>
       <c r="R150" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 43']</t>
+          <t>['SWL not found in the page', 'page no: 44']</t>
         </is>
       </c>
     </row>
@@ -8255,7 +8255,7 @@
       </c>
       <c r="R151" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 43']</t>
+          <t>['SWL not found in the page', 'page no: 44']</t>
         </is>
       </c>
     </row>
@@ -8302,7 +8302,7 @@
       </c>
       <c r="R152" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 43']</t>
+          <t>['SWL not found in the page', 'page no: 44']</t>
         </is>
       </c>
     </row>
@@ -8349,7 +8349,7 @@
       </c>
       <c r="R153" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 43']</t>
+          <t>['SWL not found in the page', 'page no: 44']</t>
         </is>
       </c>
     </row>
@@ -8396,7 +8396,7 @@
       </c>
       <c r="R154" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 43']</t>
+          <t>['SWL not found in the page', 'page no: 44']</t>
         </is>
       </c>
     </row>
@@ -8443,7 +8443,7 @@
       </c>
       <c r="R155" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 43']</t>
+          <t>['SWL not found in the page', 'page no: 44']</t>
         </is>
       </c>
     </row>
@@ -8490,7 +8490,7 @@
       </c>
       <c r="R156" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 43']</t>
+          <t>['SWL not found in the page', 'page no: 44']</t>
         </is>
       </c>
     </row>
@@ -8537,7 +8537,7 @@
       </c>
       <c r="R157" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 43']</t>
+          <t>['SWL not found in the page', 'page no: 44']</t>
         </is>
       </c>
     </row>
@@ -8584,7 +8584,7 @@
       </c>
       <c r="R158" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 43']</t>
+          <t>['SWL not found in the page', 'page no: 44']</t>
         </is>
       </c>
     </row>
@@ -8631,7 +8631,7 @@
       </c>
       <c r="R159" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 43']</t>
+          <t>['SWL not found in the page', 'page no: 44']</t>
         </is>
       </c>
     </row>
@@ -8678,7 +8678,7 @@
       </c>
       <c r="R160" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 43']</t>
+          <t>['SWL not found in the page', 'page no: 44']</t>
         </is>
       </c>
     </row>
@@ -8725,7 +8725,7 @@
       </c>
       <c r="R161" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 43']</t>
+          <t>['SWL not found in the page', 'page no: 44']</t>
         </is>
       </c>
     </row>
@@ -8772,7 +8772,7 @@
       </c>
       <c r="R162" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 43']</t>
+          <t>['SWL not found in the page', 'page no: 44']</t>
         </is>
       </c>
     </row>
@@ -8822,7 +8822,7 @@
       </c>
       <c r="R163" t="inlineStr">
         <is>
-          <t>['SWL Value not found', 'SWL Unit not found', 'page no: 44']</t>
+          <t>['SWL Value not found', 'SWL Unit not found', 'page no: 45']</t>
         </is>
       </c>
     </row>
@@ -8873,7 +8873,7 @@
       </c>
       <c r="R164" t="inlineStr">
         <is>
-          <t>['SWL Value not found', 'SWL Unit not found', 'page no: 44']</t>
+          <t>['SWL Value not found', 'SWL Unit not found', 'page no: 45']</t>
         </is>
       </c>
     </row>
@@ -8924,7 +8924,7 @@
       </c>
       <c r="R165" t="inlineStr">
         <is>
-          <t>['SWL Value not found', 'SWL Unit not found', 'page no: 44']</t>
+          <t>['SWL Value not found', 'SWL Unit not found', 'page no: 45']</t>
         </is>
       </c>
     </row>
@@ -8975,7 +8975,7 @@
       </c>
       <c r="R166" t="inlineStr">
         <is>
-          <t>['SWL Value not found', 'SWL Unit not found', 'page no: 44']</t>
+          <t>['SWL Value not found', 'SWL Unit not found', 'page no: 45']</t>
         </is>
       </c>
     </row>
@@ -9022,7 +9022,7 @@
       </c>
       <c r="R167" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 45']</t>
+          <t>['SWL not found in the page', 'page no: 46']</t>
         </is>
       </c>
     </row>
@@ -9069,7 +9069,7 @@
       </c>
       <c r="R168" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 45']</t>
+          <t>['SWL not found in the page', 'page no: 46']</t>
         </is>
       </c>
     </row>
@@ -9116,7 +9116,7 @@
       </c>
       <c r="R169" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 45']</t>
+          <t>['SWL not found in the page', 'page no: 46']</t>
         </is>
       </c>
     </row>
@@ -9163,7 +9163,7 @@
       </c>
       <c r="R170" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 45']</t>
+          <t>['SWL not found in the page', 'page no: 46']</t>
         </is>
       </c>
     </row>
@@ -9210,7 +9210,7 @@
       </c>
       <c r="R171" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 45']</t>
+          <t>['SWL not found in the page', 'page no: 46']</t>
         </is>
       </c>
     </row>
@@ -9257,7 +9257,7 @@
       </c>
       <c r="R172" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 45']</t>
+          <t>['SWL not found in the page', 'page no: 46']</t>
         </is>
       </c>
     </row>
@@ -9304,7 +9304,7 @@
       </c>
       <c r="R173" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 45']</t>
+          <t>['SWL not found in the page', 'page no: 46']</t>
         </is>
       </c>
     </row>
@@ -9351,7 +9351,7 @@
       </c>
       <c r="R174" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 45']</t>
+          <t>['SWL not found in the page', 'page no: 46']</t>
         </is>
       </c>
     </row>
@@ -9398,7 +9398,7 @@
       </c>
       <c r="R175" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 45']</t>
+          <t>['SWL not found in the page', 'page no: 46']</t>
         </is>
       </c>
     </row>
@@ -9445,7 +9445,7 @@
       </c>
       <c r="R176" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 45']</t>
+          <t>['SWL not found in the page', 'page no: 46']</t>
         </is>
       </c>
     </row>
@@ -9492,7 +9492,7 @@
       </c>
       <c r="R177" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 45']</t>
+          <t>['SWL not found in the page', 'page no: 46']</t>
         </is>
       </c>
     </row>
@@ -9539,7 +9539,7 @@
       </c>
       <c r="R178" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 45']</t>
+          <t>['SWL not found in the page', 'page no: 46']</t>
         </is>
       </c>
     </row>
@@ -9586,7 +9586,7 @@
       </c>
       <c r="R179" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 45']</t>
+          <t>['SWL not found in the page', 'page no: 46']</t>
         </is>
       </c>
     </row>
@@ -9633,7 +9633,7 @@
       </c>
       <c r="R180" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 45']</t>
+          <t>['SWL not found in the page', 'page no: 46']</t>
         </is>
       </c>
     </row>
@@ -9680,7 +9680,7 @@
       </c>
       <c r="R181" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 45']</t>
+          <t>['SWL not found in the page', 'page no: 46']</t>
         </is>
       </c>
     </row>
@@ -9727,7 +9727,7 @@
       </c>
       <c r="R182" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 45']</t>
+          <t>['SWL not found in the page', 'page no: 46']</t>
         </is>
       </c>
     </row>
@@ -9767,7 +9767,7 @@
       </c>
       <c r="R183" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 46']</t>
+          <t>['Manufacturer not found', 'SWL not found in the page', 'page no: 47']</t>
         </is>
       </c>
     </row>
@@ -9808,7 +9808,7 @@
       </c>
       <c r="R184" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 46']</t>
+          <t>['Manufacturer not found', 'SWL not found in the page', 'page no: 47']</t>
         </is>
       </c>
     </row>
@@ -9849,7 +9849,7 @@
       </c>
       <c r="R185" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 46']</t>
+          <t>['Manufacturer not found', 'SWL not found in the page', 'page no: 47']</t>
         </is>
       </c>
     </row>
@@ -9896,7 +9896,7 @@
       </c>
       <c r="R186" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 47']</t>
+          <t>['SWL not found in the page', 'page no: 48']</t>
         </is>
       </c>
     </row>
@@ -9944,7 +9944,7 @@
       </c>
       <c r="R187" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 47']</t>
+          <t>['SWL not found in the page', 'page no: 48']</t>
         </is>
       </c>
     </row>
@@ -9992,7 +9992,7 @@
       </c>
       <c r="R188" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 47']</t>
+          <t>['SWL not found in the page', 'page no: 48']</t>
         </is>
       </c>
     </row>
@@ -10039,7 +10039,7 @@
       </c>
       <c r="R189" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 48']</t>
+          <t>['SWL not found in the page', 'page no: 49']</t>
         </is>
       </c>
     </row>
@@ -10087,7 +10087,7 @@
       </c>
       <c r="R190" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 48']</t>
+          <t>['SWL not found in the page', 'page no: 49']</t>
         </is>
       </c>
     </row>
@@ -10135,7 +10135,7 @@
       </c>
       <c r="R191" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 48']</t>
+          <t>['SWL not found in the page', 'page no: 49']</t>
         </is>
       </c>
     </row>
@@ -10182,7 +10182,7 @@
       </c>
       <c r="R192" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 49']</t>
+          <t>['SWL not found in the page', 'page no: 50']</t>
         </is>
       </c>
     </row>
@@ -10230,7 +10230,7 @@
       </c>
       <c r="R193" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 49']</t>
+          <t>['SWL not found in the page', 'page no: 50']</t>
         </is>
       </c>
     </row>
@@ -10277,7 +10277,7 @@
       </c>
       <c r="R194" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 49']</t>
+          <t>['SWL not found in the page', 'page no: 50']</t>
         </is>
       </c>
     </row>
@@ -10324,7 +10324,7 @@
       </c>
       <c r="R195" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 50']</t>
+          <t>['SWL not found in the page', 'page no: 51']</t>
         </is>
       </c>
     </row>
@@ -10371,7 +10371,7 @@
       </c>
       <c r="R196" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 50']</t>
+          <t>['SWL not found in the page', 'page no: 51']</t>
         </is>
       </c>
     </row>
@@ -10419,7 +10419,7 @@
       </c>
       <c r="R197" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 50']</t>
+          <t>['SWL not found in the page', 'page no: 51']</t>
         </is>
       </c>
     </row>
@@ -10466,7 +10466,7 @@
       </c>
       <c r="R198" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 50']</t>
+          <t>['SWL not found in the page', 'page no: 51']</t>
         </is>
       </c>
     </row>
@@ -10514,7 +10514,7 @@
       </c>
       <c r="R199" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 50']</t>
+          <t>['SWL not found in the page', 'page no: 51']</t>
         </is>
       </c>
     </row>
@@ -10561,7 +10561,7 @@
       </c>
       <c r="R200" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 50']</t>
+          <t>['SWL not found in the page', 'page no: 51']</t>
         </is>
       </c>
     </row>
@@ -10609,7 +10609,7 @@
       </c>
       <c r="R201" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 50']</t>
+          <t>['SWL not found in the page', 'page no: 51']</t>
         </is>
       </c>
     </row>
@@ -10656,7 +10656,7 @@
       </c>
       <c r="R202" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 51']</t>
+          <t>['SWL not found in the page', 'page no: 52']</t>
         </is>
       </c>
     </row>
@@ -10703,7 +10703,7 @@
       </c>
       <c r="R203" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 51']</t>
+          <t>['SWL not found in the page', 'page no: 52']</t>
         </is>
       </c>
     </row>
@@ -10751,7 +10751,7 @@
       </c>
       <c r="R204" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 51']</t>
+          <t>['SWL not found in the page', 'page no: 52']</t>
         </is>
       </c>
     </row>
@@ -10798,7 +10798,7 @@
       </c>
       <c r="R205" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 51']</t>
+          <t>['SWL not found in the page', 'page no: 52']</t>
         </is>
       </c>
     </row>
@@ -10846,7 +10846,7 @@
       </c>
       <c r="R206" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 51']</t>
+          <t>['SWL not found in the page', 'page no: 52']</t>
         </is>
       </c>
     </row>
@@ -10893,7 +10893,7 @@
       </c>
       <c r="R207" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 51']</t>
+          <t>['SWL not found in the page', 'page no: 52']</t>
         </is>
       </c>
     </row>
@@ -10941,7 +10941,7 @@
       </c>
       <c r="R208" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 51']</t>
+          <t>['SWL not found in the page', 'page no: 52']</t>
         </is>
       </c>
     </row>
@@ -10988,7 +10988,7 @@
       </c>
       <c r="R209" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 52']</t>
+          <t>['SWL not found in the page', 'page no: 53']</t>
         </is>
       </c>
     </row>
@@ -11036,7 +11036,7 @@
       </c>
       <c r="R210" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 52']</t>
+          <t>['SWL not found in the page', 'page no: 53']</t>
         </is>
       </c>
     </row>
@@ -11084,7 +11084,7 @@
       </c>
       <c r="R211" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 52']</t>
+          <t>['SWL not found in the page', 'page no: 53']</t>
         </is>
       </c>
     </row>
@@ -11131,7 +11131,7 @@
       </c>
       <c r="R212" t="inlineStr">
         <is>
-          <t>['SWL not found in the page. SWL Value, SWL Unit, SWL Note columns are left empty', 'page no: 52']</t>
+          <t>['SWL not found in the page', 'page no: 53']</t>
         </is>
       </c>
     </row>
@@ -11179,7 +11179,7 @@
       </c>
       <c r="R213" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'Model not found', 'page no: 53']</t>
+          <t>['Manufacturer not found', 'Model not found', 'page no: 54']</t>
         </is>
       </c>
     </row>
@@ -11227,7 +11227,7 @@
       </c>
       <c r="R214" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'Model not found', 'page no: 53']</t>
+          <t>['Manufacturer not found', 'Model not found', 'page no: 54']</t>
         </is>
       </c>
     </row>
@@ -11275,7 +11275,7 @@
       </c>
       <c r="R215" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'Model not found', 'page no: 53']</t>
+          <t>['Manufacturer not found', 'Model not found', 'page no: 54']</t>
         </is>
       </c>
     </row>
@@ -11323,7 +11323,7 @@
       </c>
       <c r="R216" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'Model not found', 'page no: 53']</t>
+          <t>['Manufacturer not found', 'Model not found', 'page no: 54']</t>
         </is>
       </c>
     </row>
@@ -11371,7 +11371,7 @@
       </c>
       <c r="R217" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'Model not found', 'page no: 53']</t>
+          <t>['Manufacturer not found', 'Model not found', 'page no: 54']</t>
         </is>
       </c>
     </row>
@@ -11419,7 +11419,7 @@
       </c>
       <c r="R218" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'Model not found', 'page no: 53']</t>
+          <t>['Manufacturer not found', 'Model not found', 'page no: 54']</t>
         </is>
       </c>
     </row>
@@ -11467,7 +11467,7 @@
       </c>
       <c r="R219" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'Model not found', 'page no: 53']</t>
+          <t>['Manufacturer not found', 'Model not found', 'page no: 54']</t>
         </is>
       </c>
     </row>
@@ -11515,7 +11515,7 @@
       </c>
       <c r="R220" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'Model not found', 'page no: 53']</t>
+          <t>['Manufacturer not found', 'Model not found', 'page no: 54']</t>
         </is>
       </c>
     </row>
@@ -11563,7 +11563,7 @@
       </c>
       <c r="R221" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'Model not found', 'page no: 53']</t>
+          <t>['Manufacturer not found', 'Model not found', 'page no: 54']</t>
         </is>
       </c>
     </row>
@@ -11611,7 +11611,7 @@
       </c>
       <c r="R222" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'Model not found', 'page no: 53']</t>
+          <t>['Manufacturer not found', 'Model not found', 'page no: 54']</t>
         </is>
       </c>
     </row>
@@ -11659,7 +11659,7 @@
       </c>
       <c r="R223" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'Model not found', 'page no: 53']</t>
+          <t>['Manufacturer not found', 'Model not found', 'page no: 54']</t>
         </is>
       </c>
     </row>
@@ -11707,7 +11707,7 @@
       </c>
       <c r="R224" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'Model not found', 'page no: 53']</t>
+          <t>['Manufacturer not found', 'Model not found', 'page no: 54']</t>
         </is>
       </c>
     </row>
@@ -11755,7 +11755,7 @@
       </c>
       <c r="R225" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'Model not found', 'page no: 53']</t>
+          <t>['Manufacturer not found', 'Model not found', 'page no: 54']</t>
         </is>
       </c>
     </row>
@@ -11803,7 +11803,7 @@
       </c>
       <c r="R226" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'Model not found', 'page no: 53']</t>
+          <t>['Manufacturer not found', 'Model not found', 'page no: 54']</t>
         </is>
       </c>
     </row>
@@ -11851,7 +11851,7 @@
       </c>
       <c r="R227" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'Model not found', 'page no: 53']</t>
+          <t>['Manufacturer not found', 'Model not found', 'page no: 54']</t>
         </is>
       </c>
     </row>
@@ -11899,7 +11899,7 @@
       </c>
       <c r="R228" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'Model not found', 'page no: 53']</t>
+          <t>['Manufacturer not found', 'Model not found', 'page no: 54']</t>
         </is>
       </c>
     </row>
@@ -11947,7 +11947,7 @@
       </c>
       <c r="R229" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'Model not found', 'page no: 53']</t>
+          <t>['Manufacturer not found', 'Model not found', 'page no: 54']</t>
         </is>
       </c>
     </row>
@@ -11995,7 +11995,7 @@
       </c>
       <c r="R230" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'Model not found', 'page no: 53']</t>
+          <t>['Manufacturer not found', 'Model not found', 'page no: 54']</t>
         </is>
       </c>
     </row>
@@ -12043,7 +12043,7 @@
       </c>
       <c r="R231" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'Model not found', 'page no: 53']</t>
+          <t>['Manufacturer not found', 'Model not found', 'page no: 54']</t>
         </is>
       </c>
     </row>
@@ -12091,7 +12091,7 @@
       </c>
       <c r="R232" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'Model not found', 'page no: 53']</t>
+          <t>['Manufacturer not found', 'Model not found', 'page no: 54']</t>
         </is>
       </c>
     </row>
@@ -12139,7 +12139,7 @@
       </c>
       <c r="R233" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'Model not found', 'page no: 54']</t>
+          <t>['Manufacturer not found', 'Model not found', 'page no: 55']</t>
         </is>
       </c>
     </row>
@@ -12187,7 +12187,7 @@
       </c>
       <c r="R234" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'Model not found', 'page no: 54']</t>
+          <t>['Manufacturer not found', 'Model not found', 'page no: 55']</t>
         </is>
       </c>
     </row>
@@ -12235,7 +12235,7 @@
       </c>
       <c r="R235" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'Model not found', 'page no: 55']</t>
+          <t>['Manufacturer not found', 'Model not found', 'page no: 56']</t>
         </is>
       </c>
     </row>
@@ -12283,7 +12283,7 @@
       </c>
       <c r="R236" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'Model not found', 'page no: 55']</t>
+          <t>['Manufacturer not found', 'Model not found', 'page no: 56']</t>
         </is>
       </c>
     </row>
@@ -12331,7 +12331,7 @@
       </c>
       <c r="R237" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'Model not found', 'page no: 56']</t>
+          <t>['Manufacturer not found', 'Model not found', 'page no: 57']</t>
         </is>
       </c>
     </row>
@@ -12379,7 +12379,7 @@
       </c>
       <c r="R238" t="inlineStr">
         <is>
-          <t>['Manufacturer not found', 'Model not found', 'page no: 56']</t>
+          <t>['Manufacturer not found', 'Model not found', 'page no: 57']</t>
         </is>
       </c>
     </row>
@@ -12410,6 +12410,11 @@
         </is>
       </c>
       <c r="H239" t="inlineStr"/>
+      <c r="I239" t="inlineStr">
+        <is>
+          <t>Van Beest</t>
+        </is>
+      </c>
       <c r="J239" t="inlineStr">
         <is>
           <t>SB344142</t>
@@ -12428,11 +12433,6 @@
       <c r="Q239" t="inlineStr">
         <is>
           <t>LOFT-SJB110523</t>
-        </is>
-      </c>
-      <c r="R239" t="inlineStr">
-        <is>
-          <t>['Manufacturer not found', 'page no: 57']</t>
         </is>
       </c>
     </row>
@@ -12463,6 +12463,11 @@
         </is>
       </c>
       <c r="H240" t="inlineStr"/>
+      <c r="I240" t="inlineStr">
+        <is>
+          <t>Van Beest</t>
+        </is>
+      </c>
       <c r="J240" t="inlineStr">
         <is>
           <t>SB344142</t>
@@ -12481,11 +12486,6 @@
       <c r="Q240" t="inlineStr">
         <is>
           <t>LOFT-SJB110523</t>
-        </is>
-      </c>
-      <c r="R240" t="inlineStr">
-        <is>
-          <t>['Manufacturer not found', 'page no: 57']</t>
         </is>
       </c>
     </row>
@@ -12516,6 +12516,11 @@
         </is>
       </c>
       <c r="H241" t="inlineStr"/>
+      <c r="I241" t="inlineStr">
+        <is>
+          <t>Van Beest</t>
+        </is>
+      </c>
       <c r="J241" t="inlineStr">
         <is>
           <t>SB344142</t>
@@ -12534,11 +12539,6 @@
       <c r="Q241" t="inlineStr">
         <is>
           <t>LOFT-SJB110523</t>
-        </is>
-      </c>
-      <c r="R241" t="inlineStr">
-        <is>
-          <t>['Manufacturer not found', 'page no: 57']</t>
         </is>
       </c>
     </row>
@@ -12569,6 +12569,11 @@
         </is>
       </c>
       <c r="H242" t="inlineStr"/>
+      <c r="I242" t="inlineStr">
+        <is>
+          <t>Van Beest</t>
+        </is>
+      </c>
       <c r="J242" t="inlineStr">
         <is>
           <t>SB344142</t>
@@ -12587,11 +12592,6 @@
       <c r="Q242" t="inlineStr">
         <is>
           <t>LOFT-SJB110523</t>
-        </is>
-      </c>
-      <c r="R242" t="inlineStr">
-        <is>
-          <t>['Manufacturer not found', 'page no: 57']</t>
         </is>
       </c>
     </row>
@@ -12622,6 +12622,11 @@
         </is>
       </c>
       <c r="H243" t="inlineStr"/>
+      <c r="I243" t="inlineStr">
+        <is>
+          <t>Van Beest</t>
+        </is>
+      </c>
       <c r="J243" t="inlineStr">
         <is>
           <t>SB344142</t>
@@ -12640,11 +12645,6 @@
       <c r="Q243" t="inlineStr">
         <is>
           <t>LOFT-SJB110523</t>
-        </is>
-      </c>
-      <c r="R243" t="inlineStr">
-        <is>
-          <t>['Manufacturer not found', 'page no: 57']</t>
         </is>
       </c>
     </row>
@@ -12675,6 +12675,11 @@
         </is>
       </c>
       <c r="H244" t="inlineStr"/>
+      <c r="I244" t="inlineStr">
+        <is>
+          <t>Van Beest</t>
+        </is>
+      </c>
       <c r="J244" t="inlineStr">
         <is>
           <t>SB344142</t>
@@ -12693,11 +12698,6 @@
       <c r="Q244" t="inlineStr">
         <is>
           <t>LOFT-SJB110523</t>
-        </is>
-      </c>
-      <c r="R244" t="inlineStr">
-        <is>
-          <t>['Manufacturer not found', 'page no: 57']</t>
         </is>
       </c>
     </row>
@@ -12728,6 +12728,11 @@
         </is>
       </c>
       <c r="H245" t="inlineStr"/>
+      <c r="I245" t="inlineStr">
+        <is>
+          <t>Van Beest</t>
+        </is>
+      </c>
       <c r="J245" t="inlineStr">
         <is>
           <t>SB344142</t>
@@ -12746,11 +12751,6 @@
       <c r="Q245" t="inlineStr">
         <is>
           <t>LOFT-SJB110523</t>
-        </is>
-      </c>
-      <c r="R245" t="inlineStr">
-        <is>
-          <t>['Manufacturer not found', 'page no: 57']</t>
         </is>
       </c>
     </row>
@@ -12787,7 +12787,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -12797,7 +12797,7 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>

</xml_diff>